<commit_message>
augmented z miss calculation
</commit_message>
<xml_diff>
--- a/Shot_training_record.xlsx
+++ b/Shot_training_record.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d0a0418598b7d49c/Documents/GitHub/LearnToShoot/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="387" documentId="11_F25DC773A252ABDACC104858C1D976905BDE58EF" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{02076D55-908D-4431-BA2E-64B0F2435FC2}"/>
+  <xr:revisionPtr revIDLastSave="398" documentId="11_F25DC773A252ABDACC104858C1D976905BDE58EF" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{81FA5331-ABEE-4363-AC4D-1D349A761394}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -96,9 +96,6 @@
     <t>?</t>
   </si>
   <si>
-    <t>Column1</t>
-  </si>
-  <si>
     <t>Column2</t>
   </si>
   <si>
@@ -133,6 +130,9 @@
   </si>
   <si>
     <t>changed out battery, sounded slow</t>
+  </si>
+  <si>
+    <t>Adj Z miss</t>
   </si>
 </sst>
 </file>
@@ -174,7 +174,11 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -185,6 +189,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -213,7 +221,9 @@
     <tableColumn id="3" xr3:uid="{DCD47750-A910-4409-BD9A-99C0494C4FC7}" name="arm angle"/>
     <tableColumn id="4" xr3:uid="{3A47030F-9A3D-444F-BC4A-6ED13D576DE9}" name="x off center of hole"/>
     <tableColumn id="5" xr3:uid="{07EF5416-2C72-452B-94CA-BB1612B8264D}" name="z off hole edges"/>
-    <tableColumn id="6" xr3:uid="{45C6761A-1B3B-4BE8-A2F8-DF9DCD2CA52C}" name="Column1"/>
+    <tableColumn id="6" xr3:uid="{45C6761A-1B3B-4BE8-A2F8-DF9DCD2CA52C}" name="Adj Z miss" dataDxfId="0">
+      <calculatedColumnFormula>_xlfn.LET(_xlpm.Direction,SIGN(E2), E2+_xlpm.Direction*13/2)</calculatedColumnFormula>
+    </tableColumn>
     <tableColumn id="7" xr3:uid="{62B46294-8CBA-448D-AEE3-F691910D3B0B}" name="Column2"/>
     <tableColumn id="8" xr3:uid="{5B8FED09-90B6-455D-AF34-0EE18846A308}" name="Column3"/>
     <tableColumn id="9" xr3:uid="{14068149-4DAE-4DB4-B506-FC737B3D4D45}" name="off april tag angle"/>
@@ -687,7 +697,7 @@
   <dimension ref="A1:N60"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="K61" sqref="K61"/>
+      <selection activeCell="F3" sqref="F1:F60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -721,13 +731,13 @@
         <v>12</v>
       </c>
       <c r="F1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G1" t="s">
         <v>19</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>20</v>
-      </c>
-      <c r="H1" t="s">
-        <v>21</v>
       </c>
       <c r="I1" t="s">
         <v>7</v>
@@ -739,13 +749,13 @@
         <v>15</v>
       </c>
       <c r="L1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="M1" t="s">
+        <v>21</v>
+      </c>
+      <c r="N1" t="s">
         <v>22</v>
-      </c>
-      <c r="N1" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.3">
@@ -764,6 +774,10 @@
       <c r="E2">
         <v>25</v>
       </c>
+      <c r="F2">
+        <f t="shared" ref="F2:F33" si="0">_xlfn.LET(_xlpm.Direction,SIGN(E2), E2+_xlpm.Direction*13/2)</f>
+        <v>31.5</v>
+      </c>
       <c r="J2">
         <v>5800</v>
       </c>
@@ -793,6 +807,10 @@
       <c r="E3">
         <v>-35</v>
       </c>
+      <c r="F3">
+        <f t="shared" si="0"/>
+        <v>-41.5</v>
+      </c>
       <c r="J3">
         <v>5800</v>
       </c>
@@ -825,6 +843,10 @@
       <c r="E4">
         <v>5</v>
       </c>
+      <c r="F4">
+        <f t="shared" si="0"/>
+        <v>11.5</v>
+      </c>
       <c r="J4">
         <v>5800</v>
       </c>
@@ -857,6 +879,10 @@
       <c r="E5">
         <v>-3</v>
       </c>
+      <c r="F5">
+        <f t="shared" si="0"/>
+        <v>-9.5</v>
+      </c>
       <c r="J5">
         <v>5800</v>
       </c>
@@ -889,6 +915,10 @@
       <c r="E6">
         <v>10</v>
       </c>
+      <c r="F6">
+        <f t="shared" si="0"/>
+        <v>16.5</v>
+      </c>
       <c r="J6">
         <v>5800</v>
       </c>
@@ -921,6 +951,10 @@
       <c r="E7">
         <v>7</v>
       </c>
+      <c r="F7">
+        <f t="shared" si="0"/>
+        <v>13.5</v>
+      </c>
       <c r="J7">
         <v>5800</v>
       </c>
@@ -953,6 +987,10 @@
       <c r="E8">
         <v>-8</v>
       </c>
+      <c r="F8">
+        <f t="shared" si="0"/>
+        <v>-14.5</v>
+      </c>
       <c r="J8">
         <v>5800</v>
       </c>
@@ -985,6 +1023,10 @@
       <c r="E9">
         <v>5</v>
       </c>
+      <c r="F9">
+        <f t="shared" si="0"/>
+        <v>11.5</v>
+      </c>
       <c r="J9">
         <v>5800</v>
       </c>
@@ -1017,6 +1059,10 @@
       <c r="E10">
         <v>10</v>
       </c>
+      <c r="F10">
+        <f t="shared" si="0"/>
+        <v>16.5</v>
+      </c>
       <c r="J10">
         <v>5600</v>
       </c>
@@ -1049,6 +1095,10 @@
       <c r="E11">
         <v>2</v>
       </c>
+      <c r="F11">
+        <f t="shared" si="0"/>
+        <v>8.5</v>
+      </c>
       <c r="J11">
         <v>5600</v>
       </c>
@@ -1081,6 +1131,10 @@
       <c r="E12">
         <v>3</v>
       </c>
+      <c r="F12">
+        <f t="shared" si="0"/>
+        <v>9.5</v>
+      </c>
       <c r="G12" t="s">
         <v>16</v>
       </c>
@@ -1116,6 +1170,10 @@
       <c r="E13">
         <v>-1</v>
       </c>
+      <c r="F13">
+        <f t="shared" si="0"/>
+        <v>-7.5</v>
+      </c>
       <c r="G13" t="s">
         <v>17</v>
       </c>
@@ -1151,6 +1209,10 @@
       <c r="E14">
         <v>5</v>
       </c>
+      <c r="F14">
+        <f t="shared" si="0"/>
+        <v>11.5</v>
+      </c>
       <c r="J14">
         <v>5700</v>
       </c>
@@ -1183,6 +1245,10 @@
       <c r="E15">
         <v>2</v>
       </c>
+      <c r="F15">
+        <f t="shared" si="0"/>
+        <v>8.5</v>
+      </c>
       <c r="J15">
         <v>5700</v>
       </c>
@@ -1215,6 +1281,10 @@
       <c r="E16">
         <v>5</v>
       </c>
+      <c r="F16">
+        <f t="shared" si="0"/>
+        <v>11.5</v>
+      </c>
       <c r="J16">
         <v>5750</v>
       </c>
@@ -1247,6 +1317,10 @@
       <c r="E17">
         <v>7</v>
       </c>
+      <c r="F17">
+        <f t="shared" si="0"/>
+        <v>13.5</v>
+      </c>
       <c r="J17">
         <v>5750</v>
       </c>
@@ -1279,6 +1353,10 @@
       <c r="E18">
         <v>0</v>
       </c>
+      <c r="F18">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="J18">
         <v>5750</v>
       </c>
@@ -1311,6 +1389,10 @@
       <c r="E19">
         <v>-15</v>
       </c>
+      <c r="F19">
+        <f t="shared" si="0"/>
+        <v>-21.5</v>
+      </c>
       <c r="J19" t="s">
         <v>18</v>
       </c>
@@ -1343,6 +1425,10 @@
       <c r="E20">
         <v>-3</v>
       </c>
+      <c r="F20">
+        <f t="shared" si="0"/>
+        <v>-9.5</v>
+      </c>
       <c r="J20">
         <v>5750</v>
       </c>
@@ -1375,6 +1461,10 @@
       <c r="E21">
         <v>0</v>
       </c>
+      <c r="F21">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="J21">
         <v>5750</v>
       </c>
@@ -1407,6 +1497,10 @@
       <c r="E22">
         <v>-5</v>
       </c>
+      <c r="F22">
+        <f t="shared" si="0"/>
+        <v>-11.5</v>
+      </c>
       <c r="J22">
         <v>5750</v>
       </c>
@@ -1439,6 +1533,10 @@
       <c r="E23">
         <v>10</v>
       </c>
+      <c r="F23">
+        <f t="shared" si="0"/>
+        <v>16.5</v>
+      </c>
       <c r="J23">
         <v>5750</v>
       </c>
@@ -1471,14 +1569,27 @@
       <c r="E24">
         <v>-20</v>
       </c>
+      <c r="F24">
+        <f t="shared" si="0"/>
+        <v>-26.5</v>
+      </c>
       <c r="G24" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J24" t="s">
         <v>18</v>
       </c>
       <c r="K24" t="s">
         <v>18</v>
+      </c>
+      <c r="L24">
+        <v>50</v>
+      </c>
+      <c r="M24">
+        <v>0</v>
+      </c>
+      <c r="N24">
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.3">
@@ -1497,6 +1608,10 @@
       <c r="E25">
         <v>0</v>
       </c>
+      <c r="F25">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="J25">
         <v>5750</v>
       </c>
@@ -1529,6 +1644,10 @@
       <c r="E26">
         <v>0</v>
       </c>
+      <c r="F26">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="J26">
         <v>5750</v>
       </c>
@@ -1561,6 +1680,10 @@
       <c r="E27">
         <v>0</v>
       </c>
+      <c r="F27">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="J27">
         <v>5750</v>
       </c>
@@ -1593,6 +1716,10 @@
       <c r="E28">
         <v>0</v>
       </c>
+      <c r="F28">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="J28">
         <v>5750</v>
       </c>
@@ -1625,8 +1752,12 @@
       <c r="E29">
         <v>-55</v>
       </c>
+      <c r="F29">
+        <f t="shared" si="0"/>
+        <v>-61.5</v>
+      </c>
       <c r="G29" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="J29">
         <v>5750</v>
@@ -1660,6 +1791,10 @@
       <c r="E30">
         <v>3</v>
       </c>
+      <c r="F30">
+        <f t="shared" si="0"/>
+        <v>9.5</v>
+      </c>
       <c r="J30">
         <v>5750</v>
       </c>
@@ -1692,6 +1827,10 @@
       <c r="E31">
         <v>3</v>
       </c>
+      <c r="F31">
+        <f t="shared" si="0"/>
+        <v>9.5</v>
+      </c>
       <c r="J31">
         <v>5750</v>
       </c>
@@ -1724,6 +1863,10 @@
       <c r="E32">
         <v>2</v>
       </c>
+      <c r="F32">
+        <f t="shared" si="0"/>
+        <v>8.5</v>
+      </c>
       <c r="J32">
         <v>5750</v>
       </c>
@@ -1756,6 +1899,10 @@
       <c r="E33">
         <v>-5</v>
       </c>
+      <c r="F33">
+        <f t="shared" si="0"/>
+        <v>-11.5</v>
+      </c>
       <c r="J33">
         <v>5750</v>
       </c>
@@ -1788,6 +1935,10 @@
       <c r="E34">
         <v>0</v>
       </c>
+      <c r="F34">
+        <f t="shared" ref="F34:F65" si="1">_xlfn.LET(_xlpm.Direction,SIGN(E34), E34+_xlpm.Direction*13/2)</f>
+        <v>0</v>
+      </c>
       <c r="J34">
         <v>5750</v>
       </c>
@@ -1820,6 +1971,10 @@
       <c r="E35">
         <v>1</v>
       </c>
+      <c r="F35">
+        <f t="shared" si="1"/>
+        <v>7.5</v>
+      </c>
       <c r="J35">
         <v>5750</v>
       </c>
@@ -1852,6 +2007,10 @@
       <c r="E36">
         <v>-7</v>
       </c>
+      <c r="F36">
+        <f t="shared" si="1"/>
+        <v>-13.5</v>
+      </c>
       <c r="J36">
         <v>5750</v>
       </c>
@@ -1884,6 +2043,10 @@
       <c r="E37">
         <v>0</v>
       </c>
+      <c r="F37">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
       <c r="J37">
         <v>5750</v>
       </c>
@@ -1916,8 +2079,12 @@
       <c r="E38">
         <v>0</v>
       </c>
+      <c r="F38">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
       <c r="G38" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="J38">
         <v>5750</v>
@@ -1951,8 +2118,12 @@
       <c r="E39">
         <v>0</v>
       </c>
+      <c r="F39">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
       <c r="G39" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="J39">
         <v>5750</v>
@@ -1986,8 +2157,12 @@
       <c r="E40">
         <v>-4</v>
       </c>
+      <c r="F40">
+        <f t="shared" si="1"/>
+        <v>-10.5</v>
+      </c>
       <c r="G40" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J40">
         <v>5800</v>
@@ -2021,8 +2196,12 @@
       <c r="E41">
         <v>-1</v>
       </c>
+      <c r="F41">
+        <f t="shared" si="1"/>
+        <v>-7.5</v>
+      </c>
       <c r="G41" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J41">
         <v>5800</v>
@@ -2056,6 +2235,10 @@
       <c r="E42">
         <v>-10</v>
       </c>
+      <c r="F42">
+        <f t="shared" si="1"/>
+        <v>-16.5</v>
+      </c>
       <c r="J42">
         <v>5800</v>
       </c>
@@ -2088,6 +2271,10 @@
       <c r="E43">
         <v>0</v>
       </c>
+      <c r="F43">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
       <c r="J43">
         <v>5800</v>
       </c>
@@ -2120,6 +2307,10 @@
       <c r="E44">
         <v>-5</v>
       </c>
+      <c r="F44">
+        <f t="shared" si="1"/>
+        <v>-11.5</v>
+      </c>
       <c r="J44">
         <v>5800</v>
       </c>
@@ -2152,6 +2343,10 @@
       <c r="E45">
         <v>0</v>
       </c>
+      <c r="F45">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
       <c r="J45">
         <v>5800</v>
       </c>
@@ -2184,8 +2379,12 @@
       <c r="E46">
         <v>23</v>
       </c>
+      <c r="F46">
+        <f t="shared" si="1"/>
+        <v>29.5</v>
+      </c>
       <c r="G46" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="J46">
         <v>5800</v>
@@ -2204,6 +2403,9 @@
       </c>
     </row>
     <row r="47" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A47">
+        <v>46</v>
+      </c>
       <c r="B47">
         <v>7</v>
       </c>
@@ -2213,8 +2415,12 @@
       <c r="E47">
         <v>-70</v>
       </c>
+      <c r="F47">
+        <f t="shared" si="1"/>
+        <v>-76.5</v>
+      </c>
       <c r="G47" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J47" t="s">
         <v>18</v>
@@ -2222,8 +2428,20 @@
       <c r="K47" t="s">
         <v>18</v>
       </c>
+      <c r="L47">
+        <v>100</v>
+      </c>
+      <c r="M47">
+        <v>0</v>
+      </c>
+      <c r="N47">
+        <v>0</v>
+      </c>
     </row>
     <row r="48" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A48">
+        <v>47</v>
+      </c>
       <c r="B48">
         <v>7</v>
       </c>
@@ -2233,11 +2451,33 @@
       <c r="E48">
         <v>-80</v>
       </c>
+      <c r="F48">
+        <f t="shared" si="1"/>
+        <v>-86.5</v>
+      </c>
       <c r="G48" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="49" spans="2:11" x14ac:dyDescent="0.3">
+        <v>30</v>
+      </c>
+      <c r="J48">
+        <v>5800</v>
+      </c>
+      <c r="K48">
+        <v>5800</v>
+      </c>
+      <c r="L48">
+        <v>100</v>
+      </c>
+      <c r="M48">
+        <v>0</v>
+      </c>
+      <c r="N48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A49">
+        <v>48</v>
+      </c>
       <c r="B49">
         <v>7</v>
       </c>
@@ -2250,8 +2490,33 @@
       <c r="E49">
         <v>-100</v>
       </c>
-    </row>
-    <row r="50" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="F49">
+        <f t="shared" si="1"/>
+        <v>-106.5</v>
+      </c>
+      <c r="J49">
+        <v>5800</v>
+      </c>
+      <c r="K49">
+        <v>5800</v>
+      </c>
+      <c r="L49">
+        <v>100</v>
+      </c>
+      <c r="M49">
+        <v>0</v>
+      </c>
+      <c r="N49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A50">
+        <v>49</v>
+      </c>
+      <c r="B50">
+        <v>7</v>
+      </c>
       <c r="C50">
         <v>300</v>
       </c>
@@ -2261,11 +2526,36 @@
       <c r="E50">
         <v>3</v>
       </c>
+      <c r="F50">
+        <f t="shared" si="1"/>
+        <v>9.5</v>
+      </c>
       <c r="G50" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="51" spans="2:11" x14ac:dyDescent="0.3">
+        <v>26</v>
+      </c>
+      <c r="J50">
+        <v>5800</v>
+      </c>
+      <c r="K50">
+        <v>5800</v>
+      </c>
+      <c r="L50">
+        <v>100</v>
+      </c>
+      <c r="M50">
+        <v>0</v>
+      </c>
+      <c r="N50">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A51">
+        <v>50</v>
+      </c>
+      <c r="B51">
+        <v>7</v>
+      </c>
       <c r="C51">
         <v>300</v>
       </c>
@@ -2275,14 +2565,33 @@
       <c r="E51">
         <v>-30</v>
       </c>
+      <c r="F51">
+        <f t="shared" si="1"/>
+        <v>-36.5</v>
+      </c>
       <c r="J51">
         <v>5750</v>
       </c>
       <c r="K51">
         <v>5800</v>
       </c>
-    </row>
-    <row r="52" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="L51">
+        <v>100</v>
+      </c>
+      <c r="M51">
+        <v>0</v>
+      </c>
+      <c r="N51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A52">
+        <v>51</v>
+      </c>
+      <c r="B52">
+        <v>7</v>
+      </c>
       <c r="C52">
         <v>300</v>
       </c>
@@ -2292,8 +2601,33 @@
       <c r="E52">
         <v>-20</v>
       </c>
-    </row>
-    <row r="53" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="F52">
+        <f t="shared" si="1"/>
+        <v>-26.5</v>
+      </c>
+      <c r="J52">
+        <v>5750</v>
+      </c>
+      <c r="K52">
+        <v>5800</v>
+      </c>
+      <c r="L52">
+        <v>100</v>
+      </c>
+      <c r="M52">
+        <v>0</v>
+      </c>
+      <c r="N52">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A53">
+        <v>52</v>
+      </c>
+      <c r="B53">
+        <v>7</v>
+      </c>
       <c r="C53">
         <v>302</v>
       </c>
@@ -2303,8 +2637,33 @@
       <c r="E53">
         <v>-30</v>
       </c>
-    </row>
-    <row r="54" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="F53">
+        <f t="shared" si="1"/>
+        <v>-36.5</v>
+      </c>
+      <c r="J53">
+        <v>5750</v>
+      </c>
+      <c r="K53">
+        <v>5800</v>
+      </c>
+      <c r="L53">
+        <v>100</v>
+      </c>
+      <c r="M53">
+        <v>0</v>
+      </c>
+      <c r="N53">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A54">
+        <v>53</v>
+      </c>
+      <c r="B54">
+        <v>7</v>
+      </c>
       <c r="C54">
         <v>302</v>
       </c>
@@ -2314,8 +2673,33 @@
       <c r="E54">
         <v>-15</v>
       </c>
-    </row>
-    <row r="55" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="F54">
+        <f t="shared" si="1"/>
+        <v>-21.5</v>
+      </c>
+      <c r="J54">
+        <v>5750</v>
+      </c>
+      <c r="K54">
+        <v>5800</v>
+      </c>
+      <c r="L54">
+        <v>100</v>
+      </c>
+      <c r="M54">
+        <v>0</v>
+      </c>
+      <c r="N54">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A55">
+        <v>54</v>
+      </c>
+      <c r="B55">
+        <v>7</v>
+      </c>
       <c r="C55">
         <v>303</v>
       </c>
@@ -2325,8 +2709,33 @@
       <c r="E55">
         <v>1</v>
       </c>
-    </row>
-    <row r="56" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="F55">
+        <f t="shared" si="1"/>
+        <v>7.5</v>
+      </c>
+      <c r="J55">
+        <v>5750</v>
+      </c>
+      <c r="K55">
+        <v>5800</v>
+      </c>
+      <c r="L55">
+        <v>100</v>
+      </c>
+      <c r="M55">
+        <v>0</v>
+      </c>
+      <c r="N55">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A56">
+        <v>55</v>
+      </c>
+      <c r="B56">
+        <v>7</v>
+      </c>
       <c r="C56">
         <v>302.5</v>
       </c>
@@ -2336,8 +2745,33 @@
       <c r="E56">
         <v>1</v>
       </c>
-    </row>
-    <row r="57" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="F56">
+        <f t="shared" si="1"/>
+        <v>7.5</v>
+      </c>
+      <c r="J56">
+        <v>5750</v>
+      </c>
+      <c r="K56">
+        <v>5800</v>
+      </c>
+      <c r="L56">
+        <v>100</v>
+      </c>
+      <c r="M56">
+        <v>0</v>
+      </c>
+      <c r="N56">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A57">
+        <v>56</v>
+      </c>
+      <c r="B57">
+        <v>7</v>
+      </c>
       <c r="C57">
         <v>302.5</v>
       </c>
@@ -2347,29 +2781,132 @@
       <c r="E57">
         <v>-15</v>
       </c>
-    </row>
-    <row r="58" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="F57">
+        <f t="shared" si="1"/>
+        <v>-21.5</v>
+      </c>
+      <c r="J57">
+        <v>5750</v>
+      </c>
+      <c r="K57">
+        <v>5800</v>
+      </c>
+      <c r="L57">
+        <v>100</v>
+      </c>
+      <c r="M57">
+        <v>0</v>
+      </c>
+      <c r="N57">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A58">
+        <v>57</v>
+      </c>
+      <c r="B58">
+        <v>7</v>
+      </c>
       <c r="C58">
         <v>302.5</v>
       </c>
+      <c r="D58">
+        <v>0</v>
+      </c>
       <c r="E58">
         <v>-40</v>
       </c>
-    </row>
-    <row r="59" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="F58">
+        <f t="shared" si="1"/>
+        <v>-46.5</v>
+      </c>
+      <c r="J58">
+        <v>5750</v>
+      </c>
+      <c r="K58">
+        <v>5800</v>
+      </c>
+      <c r="L58">
+        <v>100</v>
+      </c>
+      <c r="M58">
+        <v>0</v>
+      </c>
+      <c r="N58">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A59">
+        <v>58</v>
+      </c>
+      <c r="B59">
+        <v>7</v>
+      </c>
+      <c r="C59">
+        <v>302.5</v>
+      </c>
+      <c r="D59">
+        <v>0</v>
+      </c>
       <c r="E59">
         <v>0</v>
       </c>
-    </row>
-    <row r="60" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="F59">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J59">
+        <v>5750</v>
+      </c>
+      <c r="K59">
+        <v>5800</v>
+      </c>
+      <c r="L59">
+        <v>100</v>
+      </c>
+      <c r="M59">
+        <v>0</v>
+      </c>
+      <c r="N59">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A60">
+        <v>59</v>
+      </c>
+      <c r="B60">
+        <v>7</v>
+      </c>
+      <c r="C60">
+        <v>302.5</v>
+      </c>
+      <c r="D60">
+        <v>0</v>
+      </c>
       <c r="E60">
         <v>-7</v>
       </c>
+      <c r="F60">
+        <f t="shared" si="1"/>
+        <v>-13.5</v>
+      </c>
       <c r="J60">
         <v>6250</v>
       </c>
       <c r="K60">
         <v>6250</v>
+      </c>
+      <c r="L60">
+        <v>100</v>
+      </c>
+      <c r="M60">
+        <v>0</v>
+      </c>
+      <c r="N60">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed pathag equation :)
</commit_message>
<xml_diff>
--- a/Shot_training_record.xlsx
+++ b/Shot_training_record.xlsx
@@ -1,26 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d0a0418598b7d49c/Documents/GitHub/LearnToShoot/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="864" documentId="11_F25DC773A252ABDACC104858C1D976905BDE58EF" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6187363E-FA4F-4F25-BECB-8F6EB71E7179}"/>
+  <xr:revisionPtr revIDLastSave="914" documentId="11_F25DC773A252ABDACC104858C1D976905BDE58EF" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7FE9ECA0-FED7-4CA6-B7D1-625C0C4DAA63}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="support values" sheetId="1" r:id="rId1"/>
     <sheet name="Data" sheetId="2" r:id="rId2"/>
     <sheet name="Pivot Table" sheetId="3" r:id="rId3"/>
-    <sheet name="Sheet2" sheetId="4" r:id="rId4"/>
+    <sheet name="SimpleFit" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="36" r:id="rId5"/>
+    <pivotCache cacheId="0" r:id="rId5"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="67">
   <si>
     <t>Point</t>
   </si>
@@ -99,9 +99,6 @@
   </si>
   <si>
     <t>left flap angle</t>
-  </si>
-  <si>
-    <t>right flap angle2</t>
   </si>
   <si>
     <t>sounded slow</t>
@@ -238,6 +235,15 @@
   <si>
     <t>456-461</t>
   </si>
+  <si>
+    <t>Time of Flight(s)</t>
+  </si>
+  <si>
+    <t>Robot angle</t>
+  </si>
+  <si>
+    <t>right flap angle</t>
+  </si>
 </sst>
 </file>
 
@@ -272,9 +278,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -286,7 +291,16 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="7">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
@@ -2608,7 +2622,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet2!$B$4</c:f>
+              <c:f>SimpleFit!$B$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2695,7 +2709,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet2!$A$5:$A$9</c:f>
+              <c:f>SimpleFit!$A$5:$A$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -2719,7 +2733,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet2!$B$5:$B$9</c:f>
+              <c:f>SimpleFit!$B$5:$B$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -7107,7 +7121,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{27307693-5E2C-48D8-ABB4-3694E08F4B4E}" name="PivotTable3" cacheId="36" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{27307693-5E2C-48D8-ABB4-3694E08F4B4E}" name="PivotTable3" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
   <location ref="A3:D35" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="18">
     <pivotField showAll="0"/>
@@ -7599,9 +7613,9 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{8D954CBD-8078-4181-B3CA-4BA49B8EEBA3}" name="shot_points" displayName="shot_points" ref="A1:I10" totalsRowShown="0">
-  <autoFilter ref="A1:I10" xr:uid="{8D954CBD-8078-4181-B3CA-4BA49B8EEBA3}"/>
-  <tableColumns count="9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{8D954CBD-8078-4181-B3CA-4BA49B8EEBA3}" name="shot_points" displayName="shot_points" ref="A1:J10" totalsRowShown="0">
+  <autoFilter ref="A1:J10" xr:uid="{8D954CBD-8078-4181-B3CA-4BA49B8EEBA3}"/>
+  <tableColumns count="10">
     <tableColumn id="1" xr3:uid="{A1CA755D-BECC-4EFC-B93F-4618AA2068CC}" name="Point"/>
     <tableColumn id="2" xr3:uid="{90F00FB3-4AEB-4503-90C8-E4F8186E6186}" name="radial"/>
     <tableColumn id="3" xr3:uid="{481A5778-206A-4E54-971B-0C3FBA0B638B}" name="x"/>
@@ -7613,15 +7627,18 @@
     <tableColumn id="7" xr3:uid="{B715B7A3-7445-4267-9E33-2AC3105D2870}" name="Ad_xComponent_point(m)"/>
     <tableColumn id="8" xr3:uid="{8CCE9403-A342-4B1F-8629-F492F737B24D}" name="Ad_ycomp"/>
     <tableColumn id="9" xr3:uid="{3BAC2A0A-04C2-4AD6-AB88-68606903EF5B}" name="Aangle_to_camera"/>
+    <tableColumn id="10" xr3:uid="{C1B7A119-8616-411D-AAA3-9837EA863A69}" name="Robot angle" dataDxfId="6">
+      <calculatedColumnFormula>ATAN2(shot_points[[#This Row],[y]],shot_points[[#This Row],[x]])*180/PI()</calculatedColumnFormula>
+    </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00C9805B-A5D6-496D-8B35-380BA7DCA433}" name="Data" displayName="Data" ref="A1:R140" totalsRowShown="0">
-  <autoFilter ref="A1:R140" xr:uid="{00C9805B-A5D6-496D-8B35-380BA7DCA433}"/>
-  <tableColumns count="18">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00C9805B-A5D6-496D-8B35-380BA7DCA433}" name="Data" displayName="Data" ref="A1:T140" totalsRowShown="0">
+  <autoFilter ref="A1:T140" xr:uid="{00C9805B-A5D6-496D-8B35-380BA7DCA433}"/>
+  <tableColumns count="20">
     <tableColumn id="1" xr3:uid="{D8EBDFBF-14D7-42DC-BD0B-2BB770D282D1}" name="shot number"/>
     <tableColumn id="2" xr3:uid="{7171FEB3-C7B7-4294-B8EC-A40D7D8D1CDA}" name="point"/>
     <tableColumn id="3" xr3:uid="{DCD47750-A910-4409-BD9A-99C0494C4FC7}" name="arm angle"/>
@@ -7630,7 +7647,7 @@
     <tableColumn id="9" xr3:uid="{C555B57A-7A99-407E-B673-ACF5AE8E95BE}" name="To_Side_angle (limelight)"/>
     <tableColumn id="4" xr3:uid="{3A47030F-9A3D-444F-BC4A-6ED13D576DE9}" name="x off center of hole"/>
     <tableColumn id="5" xr3:uid="{07EF5416-2C72-452B-94CA-BB1612B8264D}" name="z off hole edges"/>
-    <tableColumn id="6" xr3:uid="{45C6761A-1B3B-4BE8-A2F8-DF9DCD2CA52C}" name="Adj Z miss" dataDxfId="3">
+    <tableColumn id="6" xr3:uid="{45C6761A-1B3B-4BE8-A2F8-DF9DCD2CA52C}" name="Adj Z miss" dataDxfId="5">
       <calculatedColumnFormula>_xlfn.LET(_xlpm.Direction,SIGN(H2), H2+_xlpm.Direction*13/2)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="7" xr3:uid="{62B46294-8CBA-448D-AEE3-F691910D3B0B}" name="Notes"/>
@@ -7638,15 +7655,19 @@
     <tableColumn id="11" xr3:uid="{CB32C425-C98A-4D80-8115-4FCB45D7FF14}" name="right shooter speed"/>
     <tableColumn id="14" xr3:uid="{801CE351-6091-4385-BDE3-C728A56C3D82}" name="rpm tolerance"/>
     <tableColumn id="12" xr3:uid="{4682125B-D1AD-480C-869C-2239AD582EAF}" name="left flap angle"/>
-    <tableColumn id="13" xr3:uid="{D94A3377-E2BA-4246-9A5E-07046CB81C2E}" name="right flap angle2"/>
-    <tableColumn id="16" xr3:uid="{E4048F41-753B-47D9-8068-A9938F0C8841}" name="Point Position on field_x" dataDxfId="2">
+    <tableColumn id="13" xr3:uid="{D94A3377-E2BA-4246-9A5E-07046CB81C2E}" name="right flap angle"/>
+    <tableColumn id="16" xr3:uid="{E4048F41-753B-47D9-8068-A9938F0C8841}" name="Point Position on field_x" dataDxfId="4">
       <calculatedColumnFormula>VLOOKUP(Data[[#This Row],[point]],'support values'!$A:$D,3,FALSE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="17" xr3:uid="{71F56FB9-39EA-4718-AC65-DBC160F2EACD}" name="Point Position on field_y" dataDxfId="1">
+    <tableColumn id="17" xr3:uid="{71F56FB9-39EA-4718-AC65-DBC160F2EACD}" name="Point Position on field_y" dataDxfId="3">
       <calculatedColumnFormula>VLOOKUP(Data[[#This Row],[point]],'support values'!$A:$D,4,FALSE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="18" xr3:uid="{252ED615-17CC-4662-9952-8A306E7E6A98}" name="Expected Radial dist" dataDxfId="0">
+    <tableColumn id="18" xr3:uid="{252ED615-17CC-4662-9952-8A306E7E6A98}" name="Expected Radial dist" dataDxfId="2">
       <calculatedColumnFormula>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],2,FALSE)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="19" xr3:uid="{8105422D-217C-4958-9C20-288B91FAE046}" name="Time of Flight(s)" dataDxfId="1"/>
+    <tableColumn id="20" xr3:uid="{FF1E5CFF-37AF-4CE7-93DE-6FA816548F3D}" name="Robot angle" dataDxfId="0">
+      <calculatedColumnFormula>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],10,FALSE)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -7916,18 +7937,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J10"/>
+  <dimension ref="A1:R11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="5" max="5" width="11.88671875" customWidth="1"/>
+    <col min="9" max="9" width="12" customWidth="1"/>
+    <col min="10" max="10" width="17.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -7947,19 +7970,22 @@
         <v>8</v>
       </c>
       <c r="G1" t="s">
+        <v>45</v>
+      </c>
+      <c r="H1" t="s">
         <v>46</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>47</v>
       </c>
-      <c r="I1" t="s">
-        <v>48</v>
-      </c>
       <c r="J1" t="s">
+        <v>65</v>
+      </c>
+      <c r="K1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -7989,10 +8015,30 @@
         <v>-149</v>
       </c>
       <c r="J2">
+        <f>ATAN2(shot_points[[#This Row],[y]],shot_points[[#This Row],[x]])*180/PI()</f>
+        <v>-32.31573231189347</v>
+      </c>
+      <c r="K2">
         <v>5.25</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="N2">
+        <f>ATAN2(shot_points[[#This Row],[y]],shot_points[[#This Row],[x]])</f>
+        <v>-0.56401592903566011</v>
+      </c>
+      <c r="O2">
+        <f>N2*180/PI()</f>
+        <v>-32.31573231189347</v>
+      </c>
+      <c r="Q2">
+        <f>O2+shot_points[[#This Row],[Aangle_to_camera]]</f>
+        <v>-181.31573231189347</v>
+      </c>
+      <c r="R2">
+        <f>(180-ABS(shot_points[[#This Row],[Aangle_to_camera]]))*SIGN(shot_points[[#This Row],[Aangle_to_camera]])</f>
+        <v>-31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -8018,8 +8064,28 @@
       <c r="H3">
         <v>-0.04</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="J3">
+        <f>ATAN2(shot_points[[#This Row],[y]],shot_points[[#This Row],[x]])*180/PI()</f>
+        <v>0</v>
+      </c>
+      <c r="N3">
+        <f>ATAN2(shot_points[[#This Row],[y]],shot_points[[#This Row],[x]])</f>
+        <v>0</v>
+      </c>
+      <c r="O3">
+        <f t="shared" ref="O3:O11" si="1">N3*180/PI()</f>
+        <v>0</v>
+      </c>
+      <c r="Q3">
+        <f>O3+shot_points[[#This Row],[Aangle_to_camera]]</f>
+        <v>0</v>
+      </c>
+      <c r="R3">
+        <f>(180-ABS(shot_points[[#This Row],[Aangle_to_camera]]))*SIGN(shot_points[[#This Row],[Aangle_to_camera]])</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -8048,8 +8114,28 @@
       <c r="I4">
         <v>151</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="J4">
+        <f>ATAN2(shot_points[[#This Row],[y]],shot_points[[#This Row],[x]])*180/PI()</f>
+        <v>33.44337032276615</v>
+      </c>
+      <c r="N4">
+        <f>ATAN2(shot_points[[#This Row],[y]],shot_points[[#This Row],[x]])</f>
+        <v>0.583696925096028</v>
+      </c>
+      <c r="O4">
+        <f t="shared" si="1"/>
+        <v>33.44337032276615</v>
+      </c>
+      <c r="Q4">
+        <f>O4+shot_points[[#This Row],[Aangle_to_camera]]</f>
+        <v>184.44337032276616</v>
+      </c>
+      <c r="R4">
+        <f>(180-ABS(shot_points[[#This Row],[Aangle_to_camera]]))*SIGN(shot_points[[#This Row],[Aangle_to_camera]])</f>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -8078,8 +8164,28 @@
       <c r="I5">
         <v>158</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="J5">
+        <f>ATAN2(shot_points[[#This Row],[y]],shot_points[[#This Row],[x]])*180/PI()</f>
+        <v>18.165956529225532</v>
+      </c>
+      <c r="N5">
+        <f>ATAN2(shot_points[[#This Row],[y]],shot_points[[#This Row],[x]])</f>
+        <v>0.31705575320914703</v>
+      </c>
+      <c r="O5">
+        <f t="shared" si="1"/>
+        <v>18.165956529225532</v>
+      </c>
+      <c r="Q5">
+        <f>O5+shot_points[[#This Row],[Aangle_to_camera]]</f>
+        <v>176.16595652922553</v>
+      </c>
+      <c r="R5">
+        <f>(180-ABS(shot_points[[#This Row],[Aangle_to_camera]]))*SIGN(shot_points[[#This Row],[Aangle_to_camera]])</f>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -8108,8 +8214,28 @@
       <c r="I6">
         <v>-174</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="J6">
+        <f>ATAN2(shot_points[[#This Row],[y]],shot_points[[#This Row],[x]])*180/PI()</f>
+        <v>0</v>
+      </c>
+      <c r="N6">
+        <f>ATAN2(shot_points[[#This Row],[y]],shot_points[[#This Row],[x]])</f>
+        <v>0</v>
+      </c>
+      <c r="O6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="Q6">
+        <f>O6+shot_points[[#This Row],[Aangle_to_camera]]</f>
+        <v>-174</v>
+      </c>
+      <c r="R6">
+        <f>(180-ABS(shot_points[[#This Row],[Aangle_to_camera]]))*SIGN(shot_points[[#This Row],[Aangle_to_camera]])</f>
+        <v>-6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -8138,8 +8264,28 @@
       <c r="I7">
         <v>-156</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="J7">
+        <f>ATAN2(shot_points[[#This Row],[y]],shot_points[[#This Row],[x]])*180/PI()</f>
+        <v>-16.977218152259343</v>
+      </c>
+      <c r="N7">
+        <f>ATAN2(shot_points[[#This Row],[y]],shot_points[[#This Row],[x]])</f>
+        <v>-0.29630835458627353</v>
+      </c>
+      <c r="O7">
+        <f t="shared" si="1"/>
+        <v>-16.977218152259343</v>
+      </c>
+      <c r="Q7">
+        <f>O7+shot_points[[#This Row],[Aangle_to_camera]]</f>
+        <v>-172.97721815225935</v>
+      </c>
+      <c r="R7">
+        <f>(180-ABS(shot_points[[#This Row],[Aangle_to_camera]]))*SIGN(shot_points[[#This Row],[Aangle_to_camera]])</f>
+        <v>-24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -8159,8 +8305,28 @@
       <c r="F8" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="J8">
+        <f>ATAN2(shot_points[[#This Row],[y]],shot_points[[#This Row],[x]])*180/PI()</f>
+        <v>8.6984237470956209</v>
+      </c>
+      <c r="N8">
+        <f>ATAN2(shot_points[[#This Row],[y]],shot_points[[#This Row],[x]])</f>
+        <v>0.15181613412048114</v>
+      </c>
+      <c r="O8">
+        <f t="shared" si="1"/>
+        <v>8.6984237470956209</v>
+      </c>
+      <c r="Q8">
+        <f>O8+shot_points[[#This Row],[Aangle_to_camera]]</f>
+        <v>8.6984237470956209</v>
+      </c>
+      <c r="R8">
+        <f>(180-ABS(shot_points[[#This Row],[Aangle_to_camera]]))*SIGN(shot_points[[#This Row],[Aangle_to_camera]])</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>0</v>
       </c>
@@ -8180,8 +8346,28 @@
       <c r="F9" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="J9">
+        <f>ATAN2(shot_points[[#This Row],[y]],shot_points[[#This Row],[x]])*180/PI()</f>
+        <v>0</v>
+      </c>
+      <c r="N9">
+        <f>ATAN2(shot_points[[#This Row],[y]],shot_points[[#This Row],[x]])</f>
+        <v>0</v>
+      </c>
+      <c r="O9">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="Q9">
+        <f>O9+shot_points[[#This Row],[Aangle_to_camera]]</f>
+        <v>0</v>
+      </c>
+      <c r="R9">
+        <f>(180-ABS(shot_points[[#This Row],[Aangle_to_camera]]))*SIGN(shot_points[[#This Row],[Aangle_to_camera]])</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>8</v>
       </c>
@@ -8208,6 +8394,40 @@
       </c>
       <c r="I10">
         <v>178</v>
+      </c>
+      <c r="J10">
+        <f>ATAN2(shot_points[[#This Row],[y]],shot_points[[#This Row],[x]])*180/PI()</f>
+        <v>0</v>
+      </c>
+      <c r="N10">
+        <f>ATAN2(shot_points[[#This Row],[y]],shot_points[[#This Row],[x]])</f>
+        <v>0</v>
+      </c>
+      <c r="O10">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="Q10">
+        <f>O10+shot_points[[#This Row],[Aangle_to_camera]]</f>
+        <v>178</v>
+      </c>
+      <c r="R10">
+        <f>(180-ABS(shot_points[[#This Row],[Aangle_to_camera]]))*SIGN(shot_points[[#This Row],[Aangle_to_camera]])</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="N11" t="e">
+        <f>ATAN2(shot_points[[#This Row],[y]],shot_points[[#This Row],[x]])</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="O11" t="e">
+        <f t="shared" si="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="Q11" t="e">
+        <f>O11+shot_points[[#This Row],[Aangle_to_camera]]</f>
+        <v>#VALUE!</v>
       </c>
     </row>
   </sheetData>
@@ -8220,10 +8440,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E35640D0-24F6-4FAE-AC25-B782A3C37205}">
-  <dimension ref="A1:R140"/>
+  <dimension ref="A1:V140"/>
   <sheetViews>
-    <sheetView topLeftCell="B118" workbookViewId="0">
-      <selection activeCell="G47" sqref="G47:G48"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="T2" sqref="T2:T140"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8238,9 +8458,10 @@
     <col min="11" max="11" width="18" customWidth="1"/>
     <col min="12" max="13" width="19.109375" customWidth="1"/>
     <col min="14" max="14" width="11.109375" customWidth="1"/>
+    <col min="18" max="18" width="14.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -8251,13 +8472,13 @@
         <v>7</v>
       </c>
       <c r="D1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F1" t="s">
         <v>44</v>
-      </c>
-      <c r="F1" t="s">
-        <v>45</v>
       </c>
       <c r="G1" t="s">
         <v>10</v>
@@ -8266,10 +8487,10 @@
         <v>11</v>
       </c>
       <c r="I1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="J1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K1" t="s">
         <v>13</v>
@@ -8278,25 +8499,31 @@
         <v>14</v>
       </c>
       <c r="M1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="N1" t="s">
         <v>18</v>
       </c>
       <c r="O1" t="s">
-        <v>19</v>
+        <v>66</v>
       </c>
       <c r="P1" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q1" t="s">
         <v>40</v>
       </c>
-      <c r="Q1" t="s">
-        <v>41</v>
-      </c>
       <c r="R1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
+        <v>53</v>
+      </c>
+      <c r="S1" t="s">
+        <v>64</v>
+      </c>
+      <c r="T1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -8343,8 +8570,12 @@
         <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],2,FALSE)</f>
         <v>258</v>
       </c>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="T2">
+        <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],10,FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -8353,6 +8584,9 @@
       </c>
       <c r="C3">
         <v>300</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
       </c>
       <c r="H3">
         <v>-35</v>
@@ -8388,8 +8622,12 @@
         <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],2,FALSE)</f>
         <v>258</v>
       </c>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="T3">
+        <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],10,FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -8436,8 +8674,12 @@
         <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],2,FALSE)</f>
         <v>258</v>
       </c>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="T4">
+        <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],10,FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -8484,8 +8726,12 @@
         <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],2,FALSE)</f>
         <v>258</v>
       </c>
-    </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="T5">
+        <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],10,FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -8532,8 +8778,12 @@
         <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],2,FALSE)</f>
         <v>258</v>
       </c>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="T6">
+        <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],10,FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -8580,8 +8830,12 @@
         <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],2,FALSE)</f>
         <v>258</v>
       </c>
-    </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="T7">
+        <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],10,FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -8628,8 +8882,12 @@
         <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],2,FALSE)</f>
         <v>258</v>
       </c>
-    </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="T8">
+        <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],10,FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -8676,8 +8934,12 @@
         <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],2,FALSE)</f>
         <v>258</v>
       </c>
-    </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="T9">
+        <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],10,FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -8724,8 +8986,12 @@
         <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],2,FALSE)</f>
         <v>258</v>
       </c>
-    </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="T10">
+        <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],10,FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
@@ -8772,8 +9038,12 @@
         <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],2,FALSE)</f>
         <v>258</v>
       </c>
-    </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="T11">
+        <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],10,FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
@@ -8823,8 +9093,12 @@
         <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],2,FALSE)</f>
         <v>258</v>
       </c>
-    </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="T12">
+        <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],10,FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
@@ -8874,8 +9148,12 @@
         <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],2,FALSE)</f>
         <v>258</v>
       </c>
-    </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="T13">
+        <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],10,FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
@@ -8922,8 +9200,12 @@
         <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],2,FALSE)</f>
         <v>258</v>
       </c>
-    </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="T14">
+        <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],10,FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>14</v>
       </c>
@@ -8970,8 +9252,12 @@
         <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],2,FALSE)</f>
         <v>258</v>
       </c>
-    </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="T15">
+        <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],10,FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>15</v>
       </c>
@@ -9018,8 +9304,12 @@
         <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],2,FALSE)</f>
         <v>258</v>
       </c>
-    </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="T16">
+        <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],10,FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>16</v>
       </c>
@@ -9066,8 +9356,12 @@
         <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],2,FALSE)</f>
         <v>258</v>
       </c>
-    </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="T17">
+        <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],10,FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>17</v>
       </c>
@@ -9114,8 +9408,12 @@
         <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],2,FALSE)</f>
         <v>258</v>
       </c>
-    </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="T18">
+        <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],10,FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>18</v>
       </c>
@@ -9162,8 +9460,12 @@
         <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],2,FALSE)</f>
         <v>258</v>
       </c>
-    </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="T19">
+        <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],10,FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>19</v>
       </c>
@@ -9210,8 +9512,12 @@
         <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],2,FALSE)</f>
         <v>258</v>
       </c>
-    </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="T20">
+        <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],10,FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>20</v>
       </c>
@@ -9258,8 +9564,12 @@
         <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],2,FALSE)</f>
         <v>258</v>
       </c>
-    </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="T21">
+        <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],10,FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>21</v>
       </c>
@@ -9306,8 +9616,12 @@
         <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],2,FALSE)</f>
         <v>258</v>
       </c>
-    </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="T22">
+        <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],10,FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>22</v>
       </c>
@@ -9354,8 +9668,12 @@
         <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],2,FALSE)</f>
         <v>258</v>
       </c>
-    </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="T23">
+        <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],10,FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>23</v>
       </c>
@@ -9376,7 +9694,7 @@
         <v>-26.5</v>
       </c>
       <c r="J24" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K24" t="s">
         <v>17</v>
@@ -9405,8 +9723,12 @@
         <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],2,FALSE)</f>
         <v>258</v>
       </c>
-    </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="T24">
+        <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],10,FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>24</v>
       </c>
@@ -9453,8 +9775,12 @@
         <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],2,FALSE)</f>
         <v>258</v>
       </c>
-    </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="T25">
+        <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],10,FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>25</v>
       </c>
@@ -9501,8 +9827,12 @@
         <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],2,FALSE)</f>
         <v>91</v>
       </c>
-    </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="T26">
+        <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],10,FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>26</v>
       </c>
@@ -9549,8 +9879,12 @@
         <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],2,FALSE)</f>
         <v>91</v>
       </c>
-    </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="T27">
+        <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],10,FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>27</v>
       </c>
@@ -9597,8 +9931,12 @@
         <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],2,FALSE)</f>
         <v>91</v>
       </c>
-    </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="T28">
+        <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],10,FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>28</v>
       </c>
@@ -9619,7 +9957,7 @@
         <v>-61.5</v>
       </c>
       <c r="J29" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="K29">
         <v>5750</v>
@@ -9648,8 +9986,12 @@
         <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],2,FALSE)</f>
         <v>340</v>
       </c>
-    </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="T29">
+        <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],10,FALSE)</f>
+        <v>18.165956529225532</v>
+      </c>
+    </row>
+    <row r="30" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>29</v>
       </c>
@@ -9696,8 +10038,12 @@
         <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],2,FALSE)</f>
         <v>340</v>
       </c>
-    </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="T30">
+        <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],10,FALSE)</f>
+        <v>18.165956529225532</v>
+      </c>
+    </row>
+    <row r="31" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>30</v>
       </c>
@@ -9744,8 +10090,12 @@
         <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],2,FALSE)</f>
         <v>340</v>
       </c>
-    </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="T31">
+        <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],10,FALSE)</f>
+        <v>18.165956529225532</v>
+      </c>
+    </row>
+    <row r="32" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>31</v>
       </c>
@@ -9792,8 +10142,12 @@
         <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],2,FALSE)</f>
         <v>340</v>
       </c>
-    </row>
-    <row r="33" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="T32">
+        <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],10,FALSE)</f>
+        <v>18.165956529225532</v>
+      </c>
+    </row>
+    <row r="33" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>32</v>
       </c>
@@ -9840,8 +10194,12 @@
         <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],2,FALSE)</f>
         <v>340</v>
       </c>
-    </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="T33">
+        <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],10,FALSE)</f>
+        <v>18.165956529225532</v>
+      </c>
+    </row>
+    <row r="34" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>33</v>
       </c>
@@ -9888,8 +10246,12 @@
         <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],2,FALSE)</f>
         <v>340</v>
       </c>
-    </row>
-    <row r="35" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="T34">
+        <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],10,FALSE)</f>
+        <v>18.165956529225532</v>
+      </c>
+    </row>
+    <row r="35" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>34</v>
       </c>
@@ -9936,8 +10298,12 @@
         <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],2,FALSE)</f>
         <v>340</v>
       </c>
-    </row>
-    <row r="36" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="T35">
+        <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],10,FALSE)</f>
+        <v>18.165956529225532</v>
+      </c>
+    </row>
+    <row r="36" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>35</v>
       </c>
@@ -9984,8 +10350,12 @@
         <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],2,FALSE)</f>
         <v>340</v>
       </c>
-    </row>
-    <row r="37" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="T36">
+        <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],10,FALSE)</f>
+        <v>18.165956529225532</v>
+      </c>
+    </row>
+    <row r="37" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>36</v>
       </c>
@@ -10032,8 +10402,12 @@
         <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],2,FALSE)</f>
         <v>340</v>
       </c>
-    </row>
-    <row r="38" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="T37">
+        <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],10,FALSE)</f>
+        <v>18.165956529225532</v>
+      </c>
+    </row>
+    <row r="38" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>37</v>
       </c>
@@ -10054,7 +10428,7 @@
         <v>0</v>
       </c>
       <c r="J38" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K38">
         <v>5750</v>
@@ -10083,8 +10457,12 @@
         <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],2,FALSE)</f>
         <v>340</v>
       </c>
-    </row>
-    <row r="39" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="T38">
+        <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],10,FALSE)</f>
+        <v>-16.977218152259343</v>
+      </c>
+    </row>
+    <row r="39" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>38</v>
       </c>
@@ -10105,7 +10483,7 @@
         <v>0</v>
       </c>
       <c r="J39" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K39">
         <v>5750</v>
@@ -10134,8 +10512,12 @@
         <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],2,FALSE)</f>
         <v>340</v>
       </c>
-    </row>
-    <row r="40" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="T39">
+        <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],10,FALSE)</f>
+        <v>-16.977218152259343</v>
+      </c>
+    </row>
+    <row r="40" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>39</v>
       </c>
@@ -10156,7 +10538,7 @@
         <v>-10.5</v>
       </c>
       <c r="J40" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K40">
         <v>5800</v>
@@ -10185,8 +10567,12 @@
         <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],2,FALSE)</f>
         <v>340</v>
       </c>
-    </row>
-    <row r="41" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="T40">
+        <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],10,FALSE)</f>
+        <v>-16.977218152259343</v>
+      </c>
+    </row>
+    <row r="41" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>40</v>
       </c>
@@ -10207,7 +10593,7 @@
         <v>-7.5</v>
       </c>
       <c r="J41" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K41">
         <v>5800</v>
@@ -10236,8 +10622,12 @@
         <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],2,FALSE)</f>
         <v>340</v>
       </c>
-    </row>
-    <row r="42" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="T41">
+        <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],10,FALSE)</f>
+        <v>-16.977218152259343</v>
+      </c>
+    </row>
+    <row r="42" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>41</v>
       </c>
@@ -10284,8 +10674,12 @@
         <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],2,FALSE)</f>
         <v>340</v>
       </c>
-    </row>
-    <row r="43" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="T42">
+        <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],10,FALSE)</f>
+        <v>-16.977218152259343</v>
+      </c>
+    </row>
+    <row r="43" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>42</v>
       </c>
@@ -10332,8 +10726,12 @@
         <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],2,FALSE)</f>
         <v>340</v>
       </c>
-    </row>
-    <row r="44" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="T43">
+        <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],10,FALSE)</f>
+        <v>-16.977218152259343</v>
+      </c>
+    </row>
+    <row r="44" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>43</v>
       </c>
@@ -10380,8 +10778,12 @@
         <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],2,FALSE)</f>
         <v>340</v>
       </c>
-    </row>
-    <row r="45" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="T44">
+        <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],10,FALSE)</f>
+        <v>-16.977218152259343</v>
+      </c>
+    </row>
+    <row r="45" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>44</v>
       </c>
@@ -10428,8 +10830,12 @@
         <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],2,FALSE)</f>
         <v>340</v>
       </c>
-    </row>
-    <row r="46" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="T45">
+        <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],10,FALSE)</f>
+        <v>-16.977218152259343</v>
+      </c>
+    </row>
+    <row r="46" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>45</v>
       </c>
@@ -10450,7 +10856,7 @@
         <v>29.5</v>
       </c>
       <c r="J46" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="K46">
         <v>5800</v>
@@ -10479,8 +10885,19 @@
         <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],2,FALSE)</f>
         <v>460</v>
       </c>
-    </row>
-    <row r="47" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S46">
+        <v>3</v>
+      </c>
+      <c r="T46">
+        <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],10,FALSE)</f>
+        <v>8.6984237470956209</v>
+      </c>
+      <c r="V46">
+        <f>Data[[#This Row],[Expected Radial dist]]/Data[[#This Row],[Time of Flight(s)]]</f>
+        <v>153.33333333333334</v>
+      </c>
+    </row>
+    <row r="47" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>46</v>
       </c>
@@ -10501,7 +10918,7 @@
         <v>-76.5</v>
       </c>
       <c r="J47" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="K47" t="s">
         <v>17</v>
@@ -10530,8 +10947,15 @@
         <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],2,FALSE)</f>
         <v>460</v>
       </c>
-    </row>
-    <row r="48" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S47">
+        <v>3</v>
+      </c>
+      <c r="T47">
+        <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],10,FALSE)</f>
+        <v>8.6984237470956209</v>
+      </c>
+    </row>
+    <row r="48" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>47</v>
       </c>
@@ -10552,7 +10976,7 @@
         <v>-86.5</v>
       </c>
       <c r="J48" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="K48">
         <v>5800</v>
@@ -10581,8 +11005,15 @@
         <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],2,FALSE)</f>
         <v>460</v>
       </c>
-    </row>
-    <row r="49" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S48">
+        <v>3</v>
+      </c>
+      <c r="T48">
+        <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],10,FALSE)</f>
+        <v>8.6984237470956209</v>
+      </c>
+    </row>
+    <row r="49" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>48</v>
       </c>
@@ -10603,7 +11034,7 @@
         <v>-106.5</v>
       </c>
       <c r="J49" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="K49">
         <v>5800</v>
@@ -10632,8 +11063,15 @@
         <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],2,FALSE)</f>
         <v>460</v>
       </c>
-    </row>
-    <row r="50" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S49">
+        <v>3</v>
+      </c>
+      <c r="T49">
+        <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],10,FALSE)</f>
+        <v>8.6984237470956209</v>
+      </c>
+    </row>
+    <row r="50" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>49</v>
       </c>
@@ -10654,7 +11092,7 @@
         <v>9.5</v>
       </c>
       <c r="J50" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="K50">
         <v>5800</v>
@@ -10683,8 +11121,15 @@
         <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],2,FALSE)</f>
         <v>460</v>
       </c>
-    </row>
-    <row r="51" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S50">
+        <v>3</v>
+      </c>
+      <c r="T50">
+        <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],10,FALSE)</f>
+        <v>8.6984237470956209</v>
+      </c>
+    </row>
+    <row r="51" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>50</v>
       </c>
@@ -10705,7 +11150,7 @@
         <v>-36.5</v>
       </c>
       <c r="J51" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="K51">
         <v>5750</v>
@@ -10734,8 +11179,15 @@
         <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],2,FALSE)</f>
         <v>460</v>
       </c>
-    </row>
-    <row r="52" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S51">
+        <v>3</v>
+      </c>
+      <c r="T51">
+        <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],10,FALSE)</f>
+        <v>8.6984237470956209</v>
+      </c>
+    </row>
+    <row r="52" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>51</v>
       </c>
@@ -10756,7 +11208,7 @@
         <v>-26.5</v>
       </c>
       <c r="J52" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="K52">
         <v>5750</v>
@@ -10785,8 +11237,15 @@
         <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],2,FALSE)</f>
         <v>460</v>
       </c>
-    </row>
-    <row r="53" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S52">
+        <v>3</v>
+      </c>
+      <c r="T52">
+        <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],10,FALSE)</f>
+        <v>8.6984237470956209</v>
+      </c>
+    </row>
+    <row r="53" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>52</v>
       </c>
@@ -10807,7 +11266,7 @@
         <v>-36.5</v>
       </c>
       <c r="J53" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="K53">
         <v>5750</v>
@@ -10836,8 +11295,15 @@
         <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],2,FALSE)</f>
         <v>460</v>
       </c>
-    </row>
-    <row r="54" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S53">
+        <v>3</v>
+      </c>
+      <c r="T53">
+        <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],10,FALSE)</f>
+        <v>8.6984237470956209</v>
+      </c>
+    </row>
+    <row r="54" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>53</v>
       </c>
@@ -10858,7 +11324,7 @@
         <v>-21.5</v>
       </c>
       <c r="J54" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="K54">
         <v>5750</v>
@@ -10887,8 +11353,15 @@
         <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],2,FALSE)</f>
         <v>460</v>
       </c>
-    </row>
-    <row r="55" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S54">
+        <v>3</v>
+      </c>
+      <c r="T54">
+        <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],10,FALSE)</f>
+        <v>8.6984237470956209</v>
+      </c>
+    </row>
+    <row r="55" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>54</v>
       </c>
@@ -10909,7 +11382,7 @@
         <v>7.5</v>
       </c>
       <c r="J55" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="K55">
         <v>5750</v>
@@ -10938,8 +11411,15 @@
         <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],2,FALSE)</f>
         <v>460</v>
       </c>
-    </row>
-    <row r="56" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S55">
+        <v>3</v>
+      </c>
+      <c r="T55">
+        <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],10,FALSE)</f>
+        <v>8.6984237470956209</v>
+      </c>
+    </row>
+    <row r="56" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>55</v>
       </c>
@@ -10960,7 +11440,7 @@
         <v>7.5</v>
       </c>
       <c r="J56" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="K56">
         <v>5750</v>
@@ -10989,8 +11469,15 @@
         <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],2,FALSE)</f>
         <v>460</v>
       </c>
-    </row>
-    <row r="57" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S56">
+        <v>3</v>
+      </c>
+      <c r="T56">
+        <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],10,FALSE)</f>
+        <v>8.6984237470956209</v>
+      </c>
+    </row>
+    <row r="57" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>56</v>
       </c>
@@ -11011,7 +11498,7 @@
         <v>-21.5</v>
       </c>
       <c r="J57" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="K57">
         <v>5750</v>
@@ -11040,8 +11527,15 @@
         <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],2,FALSE)</f>
         <v>460</v>
       </c>
-    </row>
-    <row r="58" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S57">
+        <v>3</v>
+      </c>
+      <c r="T57">
+        <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],10,FALSE)</f>
+        <v>8.6984237470956209</v>
+      </c>
+    </row>
+    <row r="58" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>57</v>
       </c>
@@ -11062,7 +11556,7 @@
         <v>-46.5</v>
       </c>
       <c r="J58" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="K58">
         <v>5750</v>
@@ -11091,8 +11585,15 @@
         <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],2,FALSE)</f>
         <v>460</v>
       </c>
-    </row>
-    <row r="59" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S58">
+        <v>3</v>
+      </c>
+      <c r="T58">
+        <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],10,FALSE)</f>
+        <v>8.6984237470956209</v>
+      </c>
+    </row>
+    <row r="59" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>58</v>
       </c>
@@ -11113,7 +11614,7 @@
         <v>0</v>
       </c>
       <c r="J59" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="K59">
         <v>5750</v>
@@ -11142,8 +11643,15 @@
         <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],2,FALSE)</f>
         <v>460</v>
       </c>
-    </row>
-    <row r="60" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S59">
+        <v>3</v>
+      </c>
+      <c r="T59">
+        <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],10,FALSE)</f>
+        <v>8.6984237470956209</v>
+      </c>
+    </row>
+    <row r="60" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>59</v>
       </c>
@@ -11164,7 +11672,7 @@
         <v>-13.5</v>
       </c>
       <c r="J60" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="K60">
         <v>6250</v>
@@ -11193,8 +11701,15 @@
         <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],2,FALSE)</f>
         <v>460</v>
       </c>
-    </row>
-    <row r="61" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S60">
+        <v>3</v>
+      </c>
+      <c r="T60">
+        <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],10,FALSE)</f>
+        <v>8.6984237470956209</v>
+      </c>
+    </row>
+    <row r="61" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>60</v>
       </c>
@@ -11215,7 +11730,7 @@
         <v>0</v>
       </c>
       <c r="J61" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K61">
         <v>5800</v>
@@ -11244,8 +11759,15 @@
         <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],2,FALSE)</f>
         <v>460</v>
       </c>
-    </row>
-    <row r="62" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S61">
+        <v>3</v>
+      </c>
+      <c r="T61">
+        <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],10,FALSE)</f>
+        <v>8.6984237470956209</v>
+      </c>
+    </row>
+    <row r="62" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>61</v>
       </c>
@@ -11292,8 +11814,15 @@
         <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],2,FALSE)</f>
         <v>460</v>
       </c>
-    </row>
-    <row r="63" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S62">
+        <v>3</v>
+      </c>
+      <c r="T62">
+        <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],10,FALSE)</f>
+        <v>8.6984237470956209</v>
+      </c>
+    </row>
+    <row r="63" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>62</v>
       </c>
@@ -11340,8 +11869,15 @@
         <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],2,FALSE)</f>
         <v>460</v>
       </c>
-    </row>
-    <row r="64" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S63">
+        <v>3</v>
+      </c>
+      <c r="T63">
+        <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],10,FALSE)</f>
+        <v>8.6984237470956209</v>
+      </c>
+    </row>
+    <row r="64" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>63</v>
       </c>
@@ -11391,8 +11927,15 @@
         <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],2,FALSE)</f>
         <v>460</v>
       </c>
-    </row>
-    <row r="65" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S64">
+        <v>3</v>
+      </c>
+      <c r="T64">
+        <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],10,FALSE)</f>
+        <v>8.6984237470956209</v>
+      </c>
+    </row>
+    <row r="65" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>64</v>
       </c>
@@ -11442,8 +11985,15 @@
         <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],2,FALSE)</f>
         <v>460</v>
       </c>
-    </row>
-    <row r="66" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S65">
+        <v>3</v>
+      </c>
+      <c r="T65">
+        <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],10,FALSE)</f>
+        <v>8.6984237470956209</v>
+      </c>
+    </row>
+    <row r="66" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>65</v>
       </c>
@@ -11493,8 +12043,15 @@
         <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],2,FALSE)</f>
         <v>460</v>
       </c>
-    </row>
-    <row r="67" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S66">
+        <v>3</v>
+      </c>
+      <c r="T66">
+        <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],10,FALSE)</f>
+        <v>8.6984237470956209</v>
+      </c>
+    </row>
+    <row r="67" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>66</v>
       </c>
@@ -11544,8 +12101,15 @@
         <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],2,FALSE)</f>
         <v>460</v>
       </c>
-    </row>
-    <row r="68" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S67">
+        <v>3</v>
+      </c>
+      <c r="T67">
+        <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],10,FALSE)</f>
+        <v>8.6984237470956209</v>
+      </c>
+    </row>
+    <row r="68" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>67</v>
       </c>
@@ -11595,8 +12159,15 @@
         <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],2,FALSE)</f>
         <v>460</v>
       </c>
-    </row>
-    <row r="69" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S68">
+        <v>3</v>
+      </c>
+      <c r="T68">
+        <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],10,FALSE)</f>
+        <v>8.6984237470956209</v>
+      </c>
+    </row>
+    <row r="69" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>68</v>
       </c>
@@ -11646,8 +12217,15 @@
         <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],2,FALSE)</f>
         <v>460</v>
       </c>
-    </row>
-    <row r="70" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S69">
+        <v>3</v>
+      </c>
+      <c r="T69">
+        <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],10,FALSE)</f>
+        <v>8.6984237470956209</v>
+      </c>
+    </row>
+    <row r="70" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>69</v>
       </c>
@@ -11671,7 +12249,7 @@
         <v>0</v>
       </c>
       <c r="J70" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="K70">
         <v>5800</v>
@@ -11700,8 +12278,15 @@
         <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],2,FALSE)</f>
         <v>460</v>
       </c>
-    </row>
-    <row r="71" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S70">
+        <v>3</v>
+      </c>
+      <c r="T70">
+        <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],10,FALSE)</f>
+        <v>8.6984237470956209</v>
+      </c>
+    </row>
+    <row r="71" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A71">
         <v>70</v>
       </c>
@@ -11725,7 +12310,7 @@
         <v>-13.5</v>
       </c>
       <c r="J71" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="K71">
         <v>5800</v>
@@ -11754,8 +12339,15 @@
         <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],2,FALSE)</f>
         <v>460</v>
       </c>
-    </row>
-    <row r="72" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S71">
+        <v>3</v>
+      </c>
+      <c r="T71">
+        <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],10,FALSE)</f>
+        <v>8.6984237470956209</v>
+      </c>
+    </row>
+    <row r="72" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A72">
         <v>71</v>
       </c>
@@ -11779,7 +12371,7 @@
         <v>27.5</v>
       </c>
       <c r="J72" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="K72">
         <v>5800</v>
@@ -11808,8 +12400,15 @@
         <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],2,FALSE)</f>
         <v>460</v>
       </c>
-    </row>
-    <row r="73" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S72">
+        <v>3</v>
+      </c>
+      <c r="T72">
+        <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],10,FALSE)</f>
+        <v>8.6984237470956209</v>
+      </c>
+    </row>
+    <row r="73" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A73">
         <v>72</v>
       </c>
@@ -11833,7 +12432,7 @@
         <v>8.5</v>
       </c>
       <c r="J73" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K73">
         <v>5800</v>
@@ -11862,8 +12461,12 @@
         <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],2,FALSE)</f>
         <v>258</v>
       </c>
-    </row>
-    <row r="74" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="T73">
+        <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],10,FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A74">
         <v>73</v>
       </c>
@@ -11887,7 +12490,7 @@
         <v>0</v>
       </c>
       <c r="J74" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K74">
         <v>5800</v>
@@ -11916,8 +12519,12 @@
         <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],2,FALSE)</f>
         <v>258</v>
       </c>
-    </row>
-    <row r="75" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="T74">
+        <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],10,FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A75">
         <v>74</v>
       </c>
@@ -11967,8 +12574,12 @@
         <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],2,FALSE)</f>
         <v>258</v>
       </c>
-    </row>
-    <row r="76" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="T75">
+        <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],10,FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A76">
         <v>75</v>
       </c>
@@ -11992,7 +12603,7 @@
         <v>8.5</v>
       </c>
       <c r="J76" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="K76">
         <v>5800</v>
@@ -12021,8 +12632,12 @@
         <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],2,FALSE)</f>
         <v>258</v>
       </c>
-    </row>
-    <row r="77" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="T76">
+        <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],10,FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A77">
         <v>76</v>
       </c>
@@ -12046,7 +12661,7 @@
         <v>0</v>
       </c>
       <c r="J77" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="K77">
         <v>5800</v>
@@ -12075,8 +12690,12 @@
         <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],2,FALSE)</f>
         <v>258</v>
       </c>
-    </row>
-    <row r="78" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="T77">
+        <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],10,FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A78">
         <v>77</v>
       </c>
@@ -12126,8 +12745,12 @@
         <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],2,FALSE)</f>
         <v>258</v>
       </c>
-    </row>
-    <row r="79" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="T78">
+        <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],10,FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A79">
         <v>78</v>
       </c>
@@ -12177,8 +12800,12 @@
         <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],2,FALSE)</f>
         <v>258</v>
       </c>
-    </row>
-    <row r="80" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="T79">
+        <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],10,FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A80">
         <v>79</v>
       </c>
@@ -12228,8 +12855,12 @@
         <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],2,FALSE)</f>
         <v>258</v>
       </c>
-    </row>
-    <row r="81" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="T80">
+        <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],10,FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A81">
         <v>80</v>
       </c>
@@ -12279,8 +12910,12 @@
         <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],2,FALSE)</f>
         <v>258</v>
       </c>
-    </row>
-    <row r="82" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="T81">
+        <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],10,FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A82">
         <v>81</v>
       </c>
@@ -12330,8 +12965,12 @@
         <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],2,FALSE)</f>
         <v>260</v>
       </c>
-    </row>
-    <row r="83" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="T82">
+        <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],10,FALSE)</f>
+        <v>33.44337032276615</v>
+      </c>
+    </row>
+    <row r="83" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A83">
         <v>82</v>
       </c>
@@ -12381,8 +13020,12 @@
         <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],2,FALSE)</f>
         <v>260</v>
       </c>
-    </row>
-    <row r="84" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="T83">
+        <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],10,FALSE)</f>
+        <v>33.44337032276615</v>
+      </c>
+    </row>
+    <row r="84" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A84">
         <v>83</v>
       </c>
@@ -12394,6 +13037,9 @@
       </c>
       <c r="D84">
         <v>308.5</v>
+      </c>
+      <c r="G84">
+        <v>0</v>
       </c>
       <c r="H84">
         <v>-7</v>
@@ -12429,8 +13075,12 @@
         <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],2,FALSE)</f>
         <v>260</v>
       </c>
-    </row>
-    <row r="85" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="T84">
+        <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],10,FALSE)</f>
+        <v>33.44337032276615</v>
+      </c>
+    </row>
+    <row r="85" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A85">
         <v>84</v>
       </c>
@@ -12480,8 +13130,12 @@
         <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],2,FALSE)</f>
         <v>260</v>
       </c>
-    </row>
-    <row r="86" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="T85">
+        <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],10,FALSE)</f>
+        <v>33.44337032276615</v>
+      </c>
+    </row>
+    <row r="86" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A86">
         <v>85</v>
       </c>
@@ -12531,8 +13185,12 @@
         <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],2,FALSE)</f>
         <v>260</v>
       </c>
-    </row>
-    <row r="87" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="T86">
+        <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],10,FALSE)</f>
+        <v>33.44337032276615</v>
+      </c>
+    </row>
+    <row r="87" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A87">
         <v>86</v>
       </c>
@@ -12582,8 +13240,12 @@
         <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],2,FALSE)</f>
         <v>260</v>
       </c>
-    </row>
-    <row r="88" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="T87">
+        <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],10,FALSE)</f>
+        <v>33.44337032276615</v>
+      </c>
+    </row>
+    <row r="88" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A88">
         <v>87</v>
       </c>
@@ -12633,8 +13295,12 @@
         <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],2,FALSE)</f>
         <v>260</v>
       </c>
-    </row>
-    <row r="89" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="T88">
+        <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],10,FALSE)</f>
+        <v>33.44337032276615</v>
+      </c>
+    </row>
+    <row r="89" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A89">
         <v>88</v>
       </c>
@@ -12684,8 +13350,12 @@
         <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],2,FALSE)</f>
         <v>260</v>
       </c>
-    </row>
-    <row r="90" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="T89">
+        <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],10,FALSE)</f>
+        <v>33.44337032276615</v>
+      </c>
+    </row>
+    <row r="90" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A90">
         <v>89</v>
       </c>
@@ -12735,8 +13405,12 @@
         <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],2,FALSE)</f>
         <v>260</v>
       </c>
-    </row>
-    <row r="91" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="T90">
+        <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],10,FALSE)</f>
+        <v>33.44337032276615</v>
+      </c>
+    </row>
+    <row r="91" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A91">
         <v>90</v>
       </c>
@@ -12786,8 +13460,12 @@
         <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],2,FALSE)</f>
         <v>260</v>
       </c>
-    </row>
-    <row r="92" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="T91">
+        <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],10,FALSE)</f>
+        <v>33.44337032276615</v>
+      </c>
+    </row>
+    <row r="92" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A92">
         <v>91</v>
       </c>
@@ -12837,8 +13515,12 @@
         <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],2,FALSE)</f>
         <v>260</v>
       </c>
-    </row>
-    <row r="93" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="T92">
+        <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],10,FALSE)</f>
+        <v>33.44337032276615</v>
+      </c>
+    </row>
+    <row r="93" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A93">
         <v>92</v>
       </c>
@@ -12888,8 +13570,12 @@
         <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],2,FALSE)</f>
         <v>260</v>
       </c>
-    </row>
-    <row r="94" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="T93">
+        <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],10,FALSE)</f>
+        <v>33.44337032276615</v>
+      </c>
+    </row>
+    <row r="94" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A94">
         <v>93</v>
       </c>
@@ -12939,8 +13625,12 @@
         <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],2,FALSE)</f>
         <v>260</v>
       </c>
-    </row>
-    <row r="95" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="T94">
+        <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],10,FALSE)</f>
+        <v>33.44337032276615</v>
+      </c>
+    </row>
+    <row r="95" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A95">
         <v>94</v>
       </c>
@@ -12990,8 +13680,12 @@
         <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],2,FALSE)</f>
         <v>260</v>
       </c>
-    </row>
-    <row r="96" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="T95">
+        <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],10,FALSE)</f>
+        <v>33.44337032276615</v>
+      </c>
+    </row>
+    <row r="96" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A96">
         <v>95</v>
       </c>
@@ -13041,8 +13735,12 @@
         <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],2,FALSE)</f>
         <v>260</v>
       </c>
-    </row>
-    <row r="97" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="T96">
+        <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],10,FALSE)</f>
+        <v>33.44337032276615</v>
+      </c>
+    </row>
+    <row r="97" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A97">
         <v>96</v>
       </c>
@@ -13092,8 +13790,12 @@
         <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],2,FALSE)</f>
         <v>260</v>
       </c>
-    </row>
-    <row r="98" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="T97">
+        <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],10,FALSE)</f>
+        <v>33.44337032276615</v>
+      </c>
+    </row>
+    <row r="98" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A98">
         <v>97</v>
       </c>
@@ -13143,8 +13845,12 @@
         <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],2,FALSE)</f>
         <v>260</v>
       </c>
-    </row>
-    <row r="99" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="T98">
+        <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],10,FALSE)</f>
+        <v>33.44337032276615</v>
+      </c>
+    </row>
+    <row r="99" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A99">
         <v>98</v>
       </c>
@@ -13194,8 +13900,12 @@
         <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],2,FALSE)</f>
         <v>259</v>
       </c>
-    </row>
-    <row r="100" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="T99">
+        <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],10,FALSE)</f>
+        <v>-32.31573231189347</v>
+      </c>
+    </row>
+    <row r="100" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A100">
         <v>99</v>
       </c>
@@ -13245,8 +13955,12 @@
         <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],2,FALSE)</f>
         <v>259</v>
       </c>
-    </row>
-    <row r="101" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="T100">
+        <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],10,FALSE)</f>
+        <v>-32.31573231189347</v>
+      </c>
+    </row>
+    <row r="101" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A101">
         <v>100</v>
       </c>
@@ -13296,8 +14010,12 @@
         <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],2,FALSE)</f>
         <v>259</v>
       </c>
-    </row>
-    <row r="102" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="T101">
+        <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],10,FALSE)</f>
+        <v>-32.31573231189347</v>
+      </c>
+    </row>
+    <row r="102" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A102">
         <v>101</v>
       </c>
@@ -13347,8 +14065,12 @@
         <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],2,FALSE)</f>
         <v>259</v>
       </c>
-    </row>
-    <row r="103" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="T102">
+        <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],10,FALSE)</f>
+        <v>-32.31573231189347</v>
+      </c>
+    </row>
+    <row r="103" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A103">
         <v>102</v>
       </c>
@@ -13398,8 +14120,12 @@
         <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],2,FALSE)</f>
         <v>259</v>
       </c>
-    </row>
-    <row r="104" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="T103">
+        <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],10,FALSE)</f>
+        <v>-32.31573231189347</v>
+      </c>
+    </row>
+    <row r="104" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A104">
         <v>103</v>
       </c>
@@ -13449,8 +14175,12 @@
         <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],2,FALSE)</f>
         <v>259</v>
       </c>
-    </row>
-    <row r="105" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="T104">
+        <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],10,FALSE)</f>
+        <v>-32.31573231189347</v>
+      </c>
+    </row>
+    <row r="105" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A105">
         <v>104</v>
       </c>
@@ -13500,8 +14230,12 @@
         <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],2,FALSE)</f>
         <v>259</v>
       </c>
-    </row>
-    <row r="106" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="T105">
+        <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],10,FALSE)</f>
+        <v>-32.31573231189347</v>
+      </c>
+    </row>
+    <row r="106" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A106">
         <v>105</v>
       </c>
@@ -13551,8 +14285,12 @@
         <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],2,FALSE)</f>
         <v>259</v>
       </c>
-    </row>
-    <row r="107" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="T106">
+        <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],10,FALSE)</f>
+        <v>-32.31573231189347</v>
+      </c>
+    </row>
+    <row r="107" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A107">
         <v>106</v>
       </c>
@@ -13602,8 +14340,12 @@
         <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],2,FALSE)</f>
         <v>259</v>
       </c>
-    </row>
-    <row r="108" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="T107">
+        <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],10,FALSE)</f>
+        <v>-32.31573231189347</v>
+      </c>
+    </row>
+    <row r="108" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A108">
         <v>107</v>
       </c>
@@ -13627,7 +14369,7 @@
         <v>0</v>
       </c>
       <c r="J108" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K108">
         <v>5800</v>
@@ -13656,8 +14398,12 @@
         <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],2,FALSE)</f>
         <v>259</v>
       </c>
-    </row>
-    <row r="109" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="T108">
+        <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],10,FALSE)</f>
+        <v>-32.31573231189347</v>
+      </c>
+    </row>
+    <row r="109" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A109">
         <v>108</v>
       </c>
@@ -13707,8 +14453,12 @@
         <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],2,FALSE)</f>
         <v>259</v>
       </c>
-    </row>
-    <row r="110" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="T109">
+        <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],10,FALSE)</f>
+        <v>-32.31573231189347</v>
+      </c>
+    </row>
+    <row r="110" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A110">
         <v>109</v>
       </c>
@@ -13758,8 +14508,12 @@
         <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],2,FALSE)</f>
         <v>259</v>
       </c>
-    </row>
-    <row r="111" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="T110">
+        <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],10,FALSE)</f>
+        <v>-32.31573231189347</v>
+      </c>
+    </row>
+    <row r="111" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A111">
         <v>110</v>
       </c>
@@ -13809,8 +14563,12 @@
         <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],2,FALSE)</f>
         <v>259</v>
       </c>
-    </row>
-    <row r="112" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="T111">
+        <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],10,FALSE)</f>
+        <v>-32.31573231189347</v>
+      </c>
+    </row>
+    <row r="112" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A112">
         <v>111</v>
       </c>
@@ -13860,8 +14618,12 @@
         <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],2,FALSE)</f>
         <v>259</v>
       </c>
-    </row>
-    <row r="113" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="T112">
+        <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],10,FALSE)</f>
+        <v>-32.31573231189347</v>
+      </c>
+    </row>
+    <row r="113" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A113">
         <v>112</v>
       </c>
@@ -13911,8 +14673,12 @@
         <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],2,FALSE)</f>
         <v>460</v>
       </c>
-    </row>
-    <row r="114" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="T113">
+        <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],10,FALSE)</f>
+        <v>8.6984237470956209</v>
+      </c>
+    </row>
+    <row r="114" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A114">
         <v>113</v>
       </c>
@@ -13962,8 +14728,12 @@
         <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],2,FALSE)</f>
         <v>460</v>
       </c>
-    </row>
-    <row r="115" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="T114">
+        <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],10,FALSE)</f>
+        <v>8.6984237470956209</v>
+      </c>
+    </row>
+    <row r="115" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A115">
         <v>114</v>
       </c>
@@ -14013,8 +14783,12 @@
         <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],2,FALSE)</f>
         <v>460</v>
       </c>
-    </row>
-    <row r="116" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="T115">
+        <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],10,FALSE)</f>
+        <v>8.6984237470956209</v>
+      </c>
+    </row>
+    <row r="116" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A116">
         <v>115</v>
       </c>
@@ -14064,8 +14838,12 @@
         <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],2,FALSE)</f>
         <v>460</v>
       </c>
-    </row>
-    <row r="117" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="T116">
+        <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],10,FALSE)</f>
+        <v>8.6984237470956209</v>
+      </c>
+    </row>
+    <row r="117" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A117">
         <v>116</v>
       </c>
@@ -14089,7 +14867,7 @@
         <v>-16.5</v>
       </c>
       <c r="J117" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="K117">
         <v>5800</v>
@@ -14118,8 +14896,12 @@
         <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],2,FALSE)</f>
         <v>460</v>
       </c>
-    </row>
-    <row r="118" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="T117">
+        <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],10,FALSE)</f>
+        <v>8.6984237470956209</v>
+      </c>
+    </row>
+    <row r="118" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A118">
         <v>117</v>
       </c>
@@ -14169,8 +14951,12 @@
         <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],2,FALSE)</f>
         <v>460</v>
       </c>
-    </row>
-    <row r="119" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="T118">
+        <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],10,FALSE)</f>
+        <v>8.6984237470956209</v>
+      </c>
+    </row>
+    <row r="119" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A119">
         <v>118</v>
       </c>
@@ -14220,8 +15006,12 @@
         <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],2,FALSE)</f>
         <v>460</v>
       </c>
-    </row>
-    <row r="120" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="T119">
+        <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],10,FALSE)</f>
+        <v>8.6984237470956209</v>
+      </c>
+    </row>
+    <row r="120" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A120">
         <v>119</v>
       </c>
@@ -14271,8 +15061,12 @@
         <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],2,FALSE)</f>
         <v>460</v>
       </c>
-    </row>
-    <row r="121" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="T120">
+        <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],10,FALSE)</f>
+        <v>8.6984237470956209</v>
+      </c>
+    </row>
+    <row r="121" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A121">
         <v>120</v>
       </c>
@@ -14322,8 +15116,12 @@
         <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],2,FALSE)</f>
         <v>460</v>
       </c>
-    </row>
-    <row r="122" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="T121">
+        <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],10,FALSE)</f>
+        <v>8.6984237470956209</v>
+      </c>
+    </row>
+    <row r="122" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A122">
         <v>121</v>
       </c>
@@ -14373,8 +15171,12 @@
         <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],2,FALSE)</f>
         <v>340</v>
       </c>
-    </row>
-    <row r="123" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="T122">
+        <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],10,FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="123" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A123">
         <v>122</v>
       </c>
@@ -14424,8 +15226,12 @@
         <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],2,FALSE)</f>
         <v>340</v>
       </c>
-    </row>
-    <row r="124" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="T123">
+        <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],10,FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="124" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A124">
         <v>123</v>
       </c>
@@ -14475,8 +15281,12 @@
         <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],2,FALSE)</f>
         <v>340</v>
       </c>
-    </row>
-    <row r="125" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="T124">
+        <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],10,FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="125" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A125">
         <v>124</v>
       </c>
@@ -14526,8 +15336,12 @@
         <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],2,FALSE)</f>
         <v>340</v>
       </c>
-    </row>
-    <row r="126" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="T125">
+        <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],10,FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="126" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A126">
         <v>125</v>
       </c>
@@ -14577,8 +15391,12 @@
         <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],2,FALSE)</f>
         <v>340</v>
       </c>
-    </row>
-    <row r="127" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="T126">
+        <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],10,FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="127" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A127">
         <v>126</v>
       </c>
@@ -14628,8 +15446,12 @@
         <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],2,FALSE)</f>
         <v>340</v>
       </c>
-    </row>
-    <row r="128" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="T127">
+        <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],10,FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="128" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A128">
         <v>127</v>
       </c>
@@ -14679,8 +15501,12 @@
         <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],2,FALSE)</f>
         <v>340</v>
       </c>
-    </row>
-    <row r="129" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="T128">
+        <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],10,FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="129" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A129">
         <v>128</v>
       </c>
@@ -14730,8 +15556,12 @@
         <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],2,FALSE)</f>
         <v>340</v>
       </c>
-    </row>
-    <row r="130" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="T129">
+        <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],10,FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="130" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A130">
         <v>129</v>
       </c>
@@ -14781,8 +15611,12 @@
         <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],2,FALSE)</f>
         <v>340</v>
       </c>
-    </row>
-    <row r="131" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="T130">
+        <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],10,FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="131" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A131">
         <v>130</v>
       </c>
@@ -14832,8 +15666,12 @@
         <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],2,FALSE)</f>
         <v>340</v>
       </c>
-    </row>
-    <row r="132" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="T131">
+        <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],10,FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="132" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A132">
         <v>131</v>
       </c>
@@ -14883,8 +15721,12 @@
         <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],2,FALSE)</f>
         <v>340</v>
       </c>
-    </row>
-    <row r="133" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="T132">
+        <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],10,FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="133" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A133">
         <v>132</v>
       </c>
@@ -14934,8 +15776,12 @@
         <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],2,FALSE)</f>
         <v>340</v>
       </c>
-    </row>
-    <row r="134" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="T133">
+        <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],10,FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="134" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A134">
         <v>133</v>
       </c>
@@ -14985,8 +15831,12 @@
         <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],2,FALSE)</f>
         <v>340</v>
       </c>
-    </row>
-    <row r="135" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="T134">
+        <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],10,FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="135" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A135">
         <v>134</v>
       </c>
@@ -15036,8 +15886,12 @@
         <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],2,FALSE)</f>
         <v>340</v>
       </c>
-    </row>
-    <row r="136" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="T135">
+        <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],10,FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="136" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A136">
         <v>135</v>
       </c>
@@ -15067,7 +15921,7 @@
         <v>-56.5</v>
       </c>
       <c r="J136" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="K136">
         <v>5800</v>
@@ -15096,8 +15950,12 @@
         <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],2,FALSE)</f>
         <v>179.07</v>
       </c>
-    </row>
-    <row r="137" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="T136">
+        <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],10,FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="137" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A137">
         <v>136</v>
       </c>
@@ -15116,7 +15974,7 @@
       <c r="H137">
         <v>0</v>
       </c>
-      <c r="I137" s="1">
+      <c r="I137">
         <f>_xlfn.LET(_xlpm.Direction,SIGN(H137), H137+_xlpm.Direction*13/2)</f>
         <v>0</v>
       </c>
@@ -15135,11 +15993,11 @@
       <c r="O137">
         <v>0</v>
       </c>
-      <c r="P137" s="1">
+      <c r="P137">
         <f>VLOOKUP(Data[[#This Row],[point]],'support values'!$A:$D,3,FALSE)</f>
         <v>0</v>
       </c>
-      <c r="Q137" s="1">
+      <c r="Q137">
         <f>VLOOKUP(Data[[#This Row],[point]],'support values'!$A:$D,4,FALSE)</f>
         <v>179.07</v>
       </c>
@@ -15147,8 +16005,12 @@
         <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],2,FALSE)</f>
         <v>179.07</v>
       </c>
-    </row>
-    <row r="138" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="T137">
+        <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],10,FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="138" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A138">
         <v>137</v>
       </c>
@@ -15167,7 +16029,7 @@
       <c r="H138">
         <v>0</v>
       </c>
-      <c r="I138" s="1">
+      <c r="I138">
         <f>_xlfn.LET(_xlpm.Direction,SIGN(H138), H138+_xlpm.Direction*13/2)</f>
         <v>0</v>
       </c>
@@ -15186,11 +16048,11 @@
       <c r="O138">
         <v>0</v>
       </c>
-      <c r="P138" s="1">
+      <c r="P138">
         <f>VLOOKUP(Data[[#This Row],[point]],'support values'!$A:$D,3,FALSE)</f>
         <v>0</v>
       </c>
-      <c r="Q138" s="1">
+      <c r="Q138">
         <f>VLOOKUP(Data[[#This Row],[point]],'support values'!$A:$D,4,FALSE)</f>
         <v>179.07</v>
       </c>
@@ -15198,8 +16060,12 @@
         <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],2,FALSE)</f>
         <v>179.07</v>
       </c>
-    </row>
-    <row r="139" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="T138">
+        <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],10,FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="139" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A139">
         <v>138</v>
       </c>
@@ -15218,7 +16084,7 @@
       <c r="H139">
         <v>0</v>
       </c>
-      <c r="I139" s="1">
+      <c r="I139">
         <f>_xlfn.LET(_xlpm.Direction,SIGN(H139), H139+_xlpm.Direction*13/2)</f>
         <v>0</v>
       </c>
@@ -15237,11 +16103,11 @@
       <c r="O139">
         <v>0</v>
       </c>
-      <c r="P139" s="1">
+      <c r="P139">
         <f>VLOOKUP(Data[[#This Row],[point]],'support values'!$A:$D,3,FALSE)</f>
         <v>0</v>
       </c>
-      <c r="Q139" s="1">
+      <c r="Q139">
         <f>VLOOKUP(Data[[#This Row],[point]],'support values'!$A:$D,4,FALSE)</f>
         <v>179.07</v>
       </c>
@@ -15249,8 +16115,12 @@
         <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],2,FALSE)</f>
         <v>179.07</v>
       </c>
-    </row>
-    <row r="140" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="T139">
+        <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],10,FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="140" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A140">
         <v>139</v>
       </c>
@@ -15269,7 +16139,7 @@
       <c r="H140">
         <v>0</v>
       </c>
-      <c r="I140" s="1">
+      <c r="I140">
         <f>_xlfn.LET(_xlpm.Direction,SIGN(H140), H140+_xlpm.Direction*13/2)</f>
         <v>0</v>
       </c>
@@ -15288,17 +16158,21 @@
       <c r="O140">
         <v>0</v>
       </c>
-      <c r="P140" s="1">
+      <c r="P140">
         <f>VLOOKUP(Data[[#This Row],[point]],'support values'!$A:$D,3,FALSE)</f>
         <v>0</v>
       </c>
-      <c r="Q140" s="1">
+      <c r="Q140">
         <f>VLOOKUP(Data[[#This Row],[point]],'support values'!$A:$D,4,FALSE)</f>
         <v>179.07</v>
       </c>
       <c r="R140">
         <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],2,FALSE)</f>
         <v>179.07</v>
+      </c>
+      <c r="T140">
+        <f>VLOOKUP(Data[[#This Row],[point]],shot_points[#All],10,FALSE)</f>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -15341,452 +16215,446 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B3" t="s">
+        <v>54</v>
+      </c>
+      <c r="C3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="B3" t="s">
-        <v>55</v>
-      </c>
-      <c r="C3" t="s">
-        <v>52</v>
-      </c>
-      <c r="D3" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="3" t="s">
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B6">
+        <v>3</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="3">
+        <v>325</v>
+      </c>
+      <c r="B7">
+        <v>3</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B8">
+        <v>5</v>
+      </c>
+      <c r="C8">
+        <v>-11.3</v>
+      </c>
+      <c r="D8">
+        <v>25.267568145747624</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" s="3">
+        <v>309</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9">
+        <v>-56.5</v>
+      </c>
+      <c r="D9" t="e">
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" s="3">
+        <v>315</v>
+      </c>
+      <c r="B10">
+        <v>4</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B11">
+        <v>64</v>
+      </c>
+      <c r="C11">
+        <v>-2.1328125</v>
+      </c>
+      <c r="D11">
+        <v>12.537955767246453</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" s="3">
+        <v>300</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12">
+        <v>-41.5</v>
+      </c>
+      <c r="D12" t="e">
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" s="3">
+        <v>302.5</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13">
+        <v>-36.5</v>
+      </c>
+      <c r="D13" t="e">
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" s="3">
+        <v>305</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14">
+        <v>-14.5</v>
+      </c>
+      <c r="D14" t="e">
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" s="3">
+        <v>306</v>
+      </c>
+      <c r="B15">
+        <v>4</v>
+      </c>
+      <c r="C15">
+        <v>-7.75</v>
+      </c>
+      <c r="D15">
+        <v>10.202123961868594</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" s="3">
+        <v>306.5</v>
+      </c>
+      <c r="B16">
+        <v>36</v>
+      </c>
+      <c r="C16">
+        <v>-4</v>
+      </c>
+      <c r="D16">
+        <v>7.3114391782427388</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" s="3">
+        <v>307</v>
+      </c>
+      <c r="B17">
+        <v>8</v>
+      </c>
+      <c r="C17">
+        <v>-0.5625</v>
+      </c>
+      <c r="D17">
+        <v>13.356211770451338</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" s="3">
+        <v>308</v>
+      </c>
+      <c r="B18">
+        <v>11</v>
+      </c>
+      <c r="C18">
+        <v>8.4090909090909083</v>
+      </c>
+      <c r="D18">
+        <v>8.8142446693354888</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" s="3">
+        <v>310</v>
+      </c>
+      <c r="B19">
+        <v>1</v>
+      </c>
+      <c r="C19">
+        <v>11.5</v>
+      </c>
+      <c r="D19" t="e">
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" s="3">
+        <v>320</v>
+      </c>
+      <c r="B20">
+        <v>1</v>
+      </c>
+      <c r="C20">
+        <v>31.5</v>
+      </c>
+      <c r="D20" t="e">
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B21">
+        <v>31</v>
+      </c>
+      <c r="C21">
+        <v>-5.225806451612903</v>
+      </c>
+      <c r="D21">
+        <v>14.353187050081374</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" s="3">
+        <v>300</v>
+      </c>
+      <c r="B22">
+        <v>1</v>
+      </c>
+      <c r="C22">
+        <v>-61.5</v>
+      </c>
+      <c r="D22" t="e">
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23" s="3">
+        <v>302</v>
+      </c>
+      <c r="B23">
+        <v>1</v>
+      </c>
+      <c r="C23">
+        <v>-11.5</v>
+      </c>
+      <c r="D23" t="e">
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24" s="3">
+        <v>302.5</v>
+      </c>
+      <c r="B24">
+        <v>12</v>
+      </c>
+      <c r="C24">
+        <v>-4.333333333333333</v>
+      </c>
+      <c r="D24">
+        <v>7.2873905210343022</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25" s="3">
+        <v>303</v>
+      </c>
+      <c r="B25">
+        <v>9</v>
+      </c>
+      <c r="C25">
+        <v>-6.2222222222222223</v>
+      </c>
+      <c r="D25">
+        <v>13.915169580154043</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A26" s="3">
+        <v>303.5</v>
+      </c>
+      <c r="B26">
+        <v>6</v>
+      </c>
+      <c r="C26">
+        <v>0</v>
+      </c>
+      <c r="D26">
+        <v>6.7082039324993694</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A27" s="3">
+        <v>305</v>
+      </c>
+      <c r="B27">
+        <v>1</v>
+      </c>
+      <c r="C27">
+        <v>9.5</v>
+      </c>
+      <c r="D27" t="e">
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A28" s="3">
+        <v>307</v>
+      </c>
+      <c r="B28">
+        <v>1</v>
+      </c>
+      <c r="C28">
+        <v>9.5</v>
+      </c>
+      <c r="D28" t="e">
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A29" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B29">
+        <v>36</v>
+      </c>
+      <c r="C29">
+        <v>-24.916666666666668</v>
+      </c>
+      <c r="D29">
+        <v>31.292742198243257</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A30" s="3">
+        <v>294</v>
+      </c>
+      <c r="B30">
+        <v>3</v>
+      </c>
+      <c r="C30">
+        <v>-89.833333333333329</v>
+      </c>
+      <c r="D30">
+        <v>15.275252316519486</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A31" s="3">
+        <v>300</v>
+      </c>
+      <c r="B31">
+        <v>25</v>
+      </c>
+      <c r="C31">
+        <v>-20.12</v>
+      </c>
+      <c r="D31">
+        <v>26.702559178226096</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A32" s="3">
+        <v>302</v>
+      </c>
+      <c r="B32">
+        <v>2</v>
+      </c>
+      <c r="C32">
+        <v>-29</v>
+      </c>
+      <c r="D32">
+        <v>10.606601717798213</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A33" s="3">
+        <v>302.5</v>
+      </c>
+      <c r="B33">
+        <v>5</v>
+      </c>
+      <c r="C33">
+        <v>-14.8</v>
+      </c>
+      <c r="D33">
+        <v>21.022606879262142</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A34" s="3">
+        <v>303</v>
+      </c>
+      <c r="B34">
+        <v>1</v>
+      </c>
+      <c r="C34">
+        <v>7.5</v>
+      </c>
+      <c r="D34" t="e">
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A35" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="B6" s="1">
-        <v>3</v>
-      </c>
-      <c r="C6" s="1">
-        <v>0</v>
-      </c>
-      <c r="D6" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" s="4">
-        <v>325</v>
-      </c>
-      <c r="B7" s="1">
-        <v>3</v>
-      </c>
-      <c r="C7" s="1">
-        <v>0</v>
-      </c>
-      <c r="D7" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="B8" s="1">
-        <v>5</v>
-      </c>
-      <c r="C8" s="1">
-        <v>-11.3</v>
-      </c>
-      <c r="D8" s="1">
-        <v>25.267568145747624</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" s="4">
-        <v>309</v>
-      </c>
-      <c r="B9" s="1">
-        <v>1</v>
-      </c>
-      <c r="C9" s="1">
-        <v>-56.5</v>
-      </c>
-      <c r="D9" s="1" t="e">
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" s="4">
-        <v>315</v>
-      </c>
-      <c r="B10" s="1">
-        <v>4</v>
-      </c>
-      <c r="C10" s="1">
-        <v>0</v>
-      </c>
-      <c r="D10" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="B11" s="1">
-        <v>64</v>
-      </c>
-      <c r="C11" s="1">
-        <v>-2.1328125</v>
-      </c>
-      <c r="D11" s="1">
-        <v>12.537955767246453</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" s="4">
-        <v>300</v>
-      </c>
-      <c r="B12" s="1">
-        <v>1</v>
-      </c>
-      <c r="C12" s="1">
-        <v>-41.5</v>
-      </c>
-      <c r="D12" s="1" t="e">
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13" s="4">
-        <v>302.5</v>
-      </c>
-      <c r="B13" s="1">
-        <v>1</v>
-      </c>
-      <c r="C13" s="1">
-        <v>-36.5</v>
-      </c>
-      <c r="D13" s="1" t="e">
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A14" s="4">
-        <v>305</v>
-      </c>
-      <c r="B14" s="1">
-        <v>1</v>
-      </c>
-      <c r="C14" s="1">
-        <v>-14.5</v>
-      </c>
-      <c r="D14" s="1" t="e">
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A15" s="4">
-        <v>306</v>
-      </c>
-      <c r="B15" s="1">
-        <v>4</v>
-      </c>
-      <c r="C15" s="1">
-        <v>-7.75</v>
-      </c>
-      <c r="D15" s="1">
-        <v>10.202123961868594</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A16" s="4">
-        <v>306.5</v>
-      </c>
-      <c r="B16" s="1">
-        <v>36</v>
-      </c>
-      <c r="C16" s="1">
-        <v>-4</v>
-      </c>
-      <c r="D16" s="1">
-        <v>7.3114391782427388</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A17" s="4">
-        <v>307</v>
-      </c>
-      <c r="B17" s="1">
-        <v>8</v>
-      </c>
-      <c r="C17" s="1">
-        <v>-0.5625</v>
-      </c>
-      <c r="D17" s="1">
-        <v>13.356211770451338</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A18" s="4">
-        <v>308</v>
-      </c>
-      <c r="B18" s="1">
-        <v>11</v>
-      </c>
-      <c r="C18" s="1">
-        <v>8.4090909090909083</v>
-      </c>
-      <c r="D18" s="1">
-        <v>8.8142446693354888</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A19" s="4">
-        <v>310</v>
-      </c>
-      <c r="B19" s="1">
-        <v>1</v>
-      </c>
-      <c r="C19" s="1">
-        <v>11.5</v>
-      </c>
-      <c r="D19" s="1" t="e">
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A20" s="4">
-        <v>320</v>
-      </c>
-      <c r="B20" s="1">
-        <v>1</v>
-      </c>
-      <c r="C20" s="1">
-        <v>31.5</v>
-      </c>
-      <c r="D20" s="1" t="e">
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A21" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="B21" s="1">
-        <v>31</v>
-      </c>
-      <c r="C21" s="1">
-        <v>-5.225806451612903</v>
-      </c>
-      <c r="D21" s="1">
-        <v>14.353187050081374</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A22" s="4">
-        <v>300</v>
-      </c>
-      <c r="B22" s="1">
-        <v>1</v>
-      </c>
-      <c r="C22" s="1">
-        <v>-61.5</v>
-      </c>
-      <c r="D22" s="1" t="e">
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A23" s="4">
-        <v>302</v>
-      </c>
-      <c r="B23" s="1">
-        <v>1</v>
-      </c>
-      <c r="C23" s="1">
-        <v>-11.5</v>
-      </c>
-      <c r="D23" s="1" t="e">
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A24" s="4">
-        <v>302.5</v>
-      </c>
-      <c r="B24" s="1">
-        <v>12</v>
-      </c>
-      <c r="C24" s="1">
-        <v>-4.333333333333333</v>
-      </c>
-      <c r="D24" s="1">
-        <v>7.2873905210343022</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A25" s="4">
-        <v>303</v>
-      </c>
-      <c r="B25" s="1">
-        <v>9</v>
-      </c>
-      <c r="C25" s="1">
-        <v>-6.2222222222222223</v>
-      </c>
-      <c r="D25" s="1">
-        <v>13.915169580154043</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A26" s="4">
-        <v>303.5</v>
-      </c>
-      <c r="B26" s="1">
-        <v>6</v>
-      </c>
-      <c r="C26" s="1">
-        <v>0</v>
-      </c>
-      <c r="D26" s="1">
-        <v>6.7082039324993694</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A27" s="4">
-        <v>305</v>
-      </c>
-      <c r="B27" s="1">
-        <v>1</v>
-      </c>
-      <c r="C27" s="1">
-        <v>9.5</v>
-      </c>
-      <c r="D27" s="1" t="e">
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A28" s="4">
-        <v>307</v>
-      </c>
-      <c r="B28" s="1">
-        <v>1</v>
-      </c>
-      <c r="C28" s="1">
-        <v>9.5</v>
-      </c>
-      <c r="D28" s="1" t="e">
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A29" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="B29" s="1">
-        <v>36</v>
-      </c>
-      <c r="C29" s="1">
-        <v>-24.916666666666668</v>
-      </c>
-      <c r="D29" s="1">
-        <v>31.292742198243257</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A30" s="4">
-        <v>294</v>
-      </c>
-      <c r="B30" s="1">
-        <v>3</v>
-      </c>
-      <c r="C30" s="1">
-        <v>-89.833333333333329</v>
-      </c>
-      <c r="D30" s="1">
-        <v>15.275252316519486</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A31" s="4">
-        <v>300</v>
-      </c>
-      <c r="B31" s="1">
-        <v>25</v>
-      </c>
-      <c r="C31" s="1">
-        <v>-20.12</v>
-      </c>
-      <c r="D31" s="1">
-        <v>26.702559178226096</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A32" s="4">
-        <v>302</v>
-      </c>
-      <c r="B32" s="1">
-        <v>2</v>
-      </c>
-      <c r="C32" s="1">
-        <v>-29</v>
-      </c>
-      <c r="D32" s="1">
-        <v>10.606601717798213</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A33" s="4">
-        <v>302.5</v>
-      </c>
-      <c r="B33" s="1">
-        <v>5</v>
-      </c>
-      <c r="C33" s="1">
-        <v>-14.8</v>
-      </c>
-      <c r="D33" s="1">
-        <v>21.022606879262142</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A34" s="4">
-        <v>303</v>
-      </c>
-      <c r="B34" s="1">
-        <v>1</v>
-      </c>
-      <c r="C34" s="1">
-        <v>7.5</v>
-      </c>
-      <c r="D34" s="1" t="e">
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A35" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="B35" s="1">
+      <c r="B35">
         <v>139</v>
       </c>
-      <c r="C35" s="1">
+      <c r="C35">
         <v>-9.0071942446043174</v>
       </c>
-      <c r="D35" s="1">
+      <c r="D35">
         <v>21.829459686090107</v>
       </c>
     </row>
@@ -15800,7 +16668,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74DDD7E0-8B02-4EB6-85AD-439E2C0A60BC}">
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
@@ -15808,20 +16676,20 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>57</v>
+      </c>
+      <c r="B4" t="s">
         <v>58</v>
-      </c>
-      <c r="B4" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
comment out the debug outputs
</commit_message>
<xml_diff>
--- a/Shot_training_record.xlsx
+++ b/Shot_training_record.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d0a0418598b7d49c/Documents/GitHub/LearnToShoot/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="914" documentId="11_F25DC773A252ABDACC104858C1D976905BDE58EF" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7FE9ECA0-FED7-4CA6-B7D1-625C0C4DAA63}"/>
+  <xr:revisionPtr revIDLastSave="923" documentId="11_F25DC773A252ABDACC104858C1D976905BDE58EF" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4BD88BE7-8EF1-4E68-9282-3133C5544F10}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="support values" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="68">
   <si>
     <t>Point</t>
   </si>
@@ -243,6 +243,9 @@
   </si>
   <si>
     <t>right flap angle</t>
+  </si>
+  <si>
+    <t>from pymc:</t>
   </si>
 </sst>
 </file>
@@ -2667,7 +2670,6 @@
             </c:spPr>
             <c:trendlineType val="poly"/>
             <c:order val="2"/>
-            <c:intercept val="339"/>
             <c:dispRSqr val="0"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
@@ -2738,19 +2740,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>325</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>315</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>307</c:v>
+                  <c:v>32</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>303.5</c:v>
+                  <c:v>28.5</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>302.75</c:v>
+                  <c:v>27.75</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4086,16 +4088,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>533400</xdr:colOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>251460</xdr:colOff>
       <xdr:row>6</xdr:row>
       <xdr:rowOff>41910</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>228600</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>41910</xdr:rowOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>99060</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4118,6 +4120,50 @@
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>488145</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>114659</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{07597B14-61DC-1184-5025-6F79F2F80203}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4876800" y="4389120"/>
+          <a:ext cx="5364945" cy="4138019"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -7939,7 +7985,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
@@ -8442,7 +8488,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E35640D0-24F6-4FAE-AC25-B782A3C37205}">
   <dimension ref="A1:V140"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="T2" sqref="T2:T140"/>
     </sheetView>
   </sheetViews>
@@ -16666,70 +16712,98 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74DDD7E0-8B02-4EB6-85AD-439E2C0A60BC}">
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:I24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>57</v>
       </c>
       <c r="B4" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C4" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>90</v>
       </c>
       <c r="B5">
+        <f>C5-275</f>
+        <v>50</v>
+      </c>
+      <c r="C5">
         <v>325</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>175</v>
       </c>
       <c r="B6">
+        <f t="shared" ref="B6:B9" si="0">C6-275</f>
+        <v>40</v>
+      </c>
+      <c r="C6">
         <v>315</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>259</v>
       </c>
       <c r="B7">
+        <f t="shared" si="0"/>
+        <v>32</v>
+      </c>
+      <c r="C7">
         <v>307</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>339</v>
       </c>
       <c r="B8">
+        <f t="shared" si="0"/>
+        <v>28.5</v>
+      </c>
+      <c r="C8">
         <v>303.5</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>459</v>
       </c>
       <c r="B9">
+        <f t="shared" si="0"/>
+        <v>27.75</v>
+      </c>
+      <c r="C9">
         <v>302.75</v>
+      </c>
+    </row>
+    <row r="24" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I24" t="s">
+        <v>67</v>
       </c>
     </row>
   </sheetData>

</xml_diff>